<commit_message>
minor adjustments to get rid of last zz's
</commit_message>
<xml_diff>
--- a/VT_REGION1_REF.xlsx
+++ b/VT_REGION1_REF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0EF47E-270D-4A44-87A4-A60BF5BCB7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28CB25-0F2D-4918-81B1-F6AA3D53C8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5340" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
+    <workbookView xWindow="405" yWindow="-16290" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -9468,6 +9468,24 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9497,24 +9515,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9552,31 +9552,10 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9595,6 +9574,27 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -18764,10 +18764,10 @@
   <dimension ref="A1:BH117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="8" topLeftCell="M97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="C71" sqref="C71:I73"/>
+      <selection pane="bottomRight" activeCell="AD116" sqref="AD116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20196,7 +20196,7 @@
       </c>
       <c r="F18" s="435">
         <f>SUMIF(RefineriesData!$J$16:$J$270,$B18&amp;F$4,RefineriesData!$N$16:$N$270)</f>
-        <v>0.95198971146726152</v>
+        <v>0.96412108310809064</v>
       </c>
       <c r="G18" s="436"/>
       <c r="H18" s="436"/>
@@ -20261,7 +20261,7 @@
       </c>
       <c r="AE18" s="435">
         <f>SUMIF(RefineriesData!$J$16:$J$270,$B18&amp;AE$3,RefineriesData!$N$16:$N$270)</f>
-        <v>190.08954718866366</v>
+        <v>192.51189158399163</v>
       </c>
       <c r="AF18" s="465"/>
       <c r="AG18" s="465"/>
@@ -20288,7 +20288,7 @@
       <c r="BB18" s="465"/>
       <c r="BC18" s="465">
         <f>AE18</f>
-        <v>190.08954718866366</v>
+        <v>192.51189158399163</v>
       </c>
       <c r="BD18" s="465">
         <v>0</v>
@@ -20368,7 +20368,7 @@
       <c r="H20" s="436"/>
       <c r="I20" s="482">
         <f>SUMIF(RefineriesData!$J$16:$J$270,B18&amp;C20,RefineriesData!$N$16:$N$270)</f>
-        <v>4.5130780547547305E-3</v>
+        <v>4.4562907610366017E-3</v>
       </c>
       <c r="J20" s="439"/>
       <c r="K20" s="435"/>
@@ -20504,7 +20504,7 @@
       </c>
       <c r="H22" s="442">
         <f>SUMIF(RefineriesData!$J$16:$J$245,$B18&amp;RIGHT($E22,3),RefineriesData!$N$16:$N$245)</f>
-        <v>0.35276939364868132</v>
+        <v>0.34833055635651694</v>
       </c>
       <c r="I22" s="442"/>
       <c r="J22" s="439"/>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="H23" s="442">
         <f>SUMIF(RefineriesData!$J$16:$J$245,$B18&amp;RIGHT($E23,3),RefineriesData!$N$16:$N$245)</f>
-        <v>0.3002204613879127</v>
+        <v>0.29644283837448704</v>
       </c>
       <c r="I23" s="442"/>
       <c r="J23" s="439"/>
@@ -20644,7 +20644,7 @@
       </c>
       <c r="H24" s="442">
         <f>SUMIF(RefineriesData!$J$16:$J$245,$B18&amp;RIGHT($E24,3),RefineriesData!$N$16:$N$245)</f>
-        <v>0.20197781416846072</v>
+        <v>0.19943636167892398</v>
       </c>
       <c r="I24" s="442"/>
       <c r="J24" s="439"/>
@@ -20714,7 +20714,7 @@
       </c>
       <c r="H25" s="442">
         <f>SUMIF(RefineriesData!$J$16:$J$245,$B18&amp;RIGHT($E25,3),RefineriesData!$N$16:$N$245)</f>
-        <v>0.12524521696188154</v>
+        <v>0.12366927769468629</v>
       </c>
       <c r="I25" s="442"/>
       <c r="J25" s="439"/>
@@ -20784,7 +20784,7 @@
       </c>
       <c r="H26" s="442">
         <f>SUMIF(RefineriesData!$J$16:$J$245,$B18&amp;RIGHT($E26,3),RefineriesData!$N$16:$N$245)</f>
-        <v>0</v>
+        <v>1.2582829950902787E-2</v>
       </c>
       <c r="I26" s="442"/>
       <c r="J26" s="439"/>
@@ -20809,7 +20809,7 @@
       <c r="AC26" s="436"/>
       <c r="AD26" s="435">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.8409817404492801</v>
       </c>
       <c r="AE26" s="465"/>
       <c r="AF26" s="465"/>
@@ -20854,7 +20854,7 @@
       </c>
       <c r="H27" s="442">
         <f>1-SUM(H21:H26)</f>
-        <v>1.9787113833063752E-2</v>
+        <v>1.9538135944483059E-2</v>
       </c>
       <c r="I27" s="442"/>
       <c r="J27" s="439"/>
@@ -20879,7 +20879,7 @@
       <c r="AC27" s="436"/>
       <c r="AD27" s="435">
         <f t="shared" si="8"/>
-        <v>2.8586058666102003</v>
+        <v>2.8586058666101857</v>
       </c>
       <c r="AE27" s="465"/>
       <c r="AF27" s="465"/>
@@ -22025,7 +22025,7 @@
       <c r="AB43" s="436"/>
       <c r="AC43" s="436"/>
       <c r="AD43" s="435">
-        <f>AD$40*F$40*H43</f>
+        <f t="shared" ref="AD43:AD48" si="12">AD$40*F$40*H43</f>
         <v>1.0986365425199789</v>
       </c>
       <c r="AE43" s="465"/>
@@ -22093,7 +22093,7 @@
       <c r="AB44" s="436"/>
       <c r="AC44" s="436"/>
       <c r="AD44" s="435">
-        <f>AD$40*F$40*H44</f>
+        <f t="shared" si="12"/>
         <v>1.6479548137799682</v>
       </c>
       <c r="AE44" s="465"/>
@@ -22161,7 +22161,7 @@
       <c r="AB45" s="436"/>
       <c r="AC45" s="436"/>
       <c r="AD45" s="435">
-        <f>AD$40*F$40*H45</f>
+        <f t="shared" si="12"/>
         <v>14.55693418838972</v>
       </c>
       <c r="AE45" s="465"/>
@@ -22229,7 +22229,7 @@
       <c r="AB46" s="436"/>
       <c r="AC46" s="436"/>
       <c r="AD46" s="435">
-        <f>AD$40*F$40*H46</f>
+        <f t="shared" si="12"/>
         <v>3.0212504919299419</v>
       </c>
       <c r="AE46" s="465"/>
@@ -22297,7 +22297,7 @@
       <c r="AB47" s="436"/>
       <c r="AC47" s="436"/>
       <c r="AD47" s="435">
-        <f>AD$40*F$40*H47</f>
+        <f t="shared" si="12"/>
         <v>2.1972730850399578</v>
       </c>
       <c r="AE47" s="465"/>
@@ -22365,7 +22365,7 @@
       <c r="AB48" s="436"/>
       <c r="AC48" s="436"/>
       <c r="AD48" s="435">
-        <f>AD$40*F$40*H48</f>
+        <f t="shared" si="12"/>
         <v>4.9438644413399047</v>
       </c>
       <c r="AE48" s="465"/>
@@ -24220,7 +24220,7 @@
       <c r="AB75" s="436"/>
       <c r="AC75" s="436"/>
       <c r="AD75" s="435">
-        <f t="shared" ref="AD75:AD80" si="12">AD$70*F$70*H75</f>
+        <f t="shared" ref="AD75:AD80" si="13">AD$70*F$70*H75</f>
         <v>53.084026088903464</v>
       </c>
       <c r="AE75" s="465"/>
@@ -24290,7 +24290,7 @@
       <c r="AB76" s="436"/>
       <c r="AC76" s="436"/>
       <c r="AD76" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>120.52809004075719</v>
       </c>
       <c r="AE76" s="465"/>
@@ -24360,7 +24360,7 @@
       <c r="AB77" s="436"/>
       <c r="AC77" s="436"/>
       <c r="AD77" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.9468278391547447</v>
       </c>
       <c r="AE77" s="465"/>
@@ -24430,7 +24430,7 @@
       <c r="AB78" s="436"/>
       <c r="AC78" s="436"/>
       <c r="AD78" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.6672857142857165</v>
       </c>
       <c r="AE78" s="465"/>
@@ -24500,7 +24500,7 @@
       <c r="AB79" s="436"/>
       <c r="AC79" s="436"/>
       <c r="AD79" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.0670273988922867</v>
       </c>
       <c r="AE79" s="465"/>
@@ -24570,7 +24570,7 @@
       <c r="AB80" s="436"/>
       <c r="AC80" s="436"/>
       <c r="AD80" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>20.5262472791314</v>
       </c>
       <c r="AE80" s="465"/>
@@ -25658,7 +25658,7 @@
       <c r="H96" s="436"/>
       <c r="I96" s="482">
         <f>SUMIF(RefineriesData!$J$16:$J$270,B94&amp;C96,RefineriesData!$N$16:$N$270)</f>
-        <v>4.5130780547547305E-3</v>
+        <v>4.4562907610366017E-3</v>
       </c>
       <c r="J96" s="439"/>
       <c r="K96" s="435"/>
@@ -26487,7 +26487,7 @@
         <v>499</v>
       </c>
       <c r="AD112" s="117">
-        <f t="shared" ref="AD112:AD117" si="13">SUMIF($E$7:$E$107,E112,$AD$7:$AD$107)</f>
+        <f t="shared" ref="AD112:AD117" si="14">SUMIF($E$7:$E$107,E112,$AD$7:$AD$107)</f>
         <v>303.09899561263535</v>
       </c>
     </row>
@@ -26496,7 +26496,7 @@
         <v>497</v>
       </c>
       <c r="AD113" s="117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>349.69632725204076</v>
       </c>
     </row>
@@ -26505,7 +26505,7 @@
         <v>491</v>
       </c>
       <c r="AD114" s="117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>135.16558341186152</v>
       </c>
     </row>
@@ -26514,7 +26514,7 @@
         <v>490</v>
       </c>
       <c r="AD115" s="117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>106.74674803946569</v>
       </c>
     </row>
@@ -26523,8 +26523,8 @@
         <v>487</v>
       </c>
       <c r="AD116" s="117">
-        <f t="shared" si="13"/>
-        <v>14.764122522740021</v>
+        <f t="shared" si="14"/>
+        <v>16.6051042631893</v>
       </c>
     </row>
     <row r="117" spans="5:30" x14ac:dyDescent="0.2">
@@ -26532,8 +26532,8 @@
         <v>485</v>
       </c>
       <c r="AD117" s="117">
-        <f t="shared" si="13"/>
-        <v>52.183618971427109</v>
+        <f t="shared" si="14"/>
+        <v>52.183618971427094</v>
       </c>
     </row>
   </sheetData>
@@ -26550,8 +26550,8 @@
   </sheetPr>
   <dimension ref="A1:AH286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31024,7 +31024,7 @@
       </c>
       <c r="N181" s="481">
         <f>D182/D193</f>
-        <v>4.5130780547547305E-3</v>
+        <v>4.4562907610366017E-3</v>
       </c>
     </row>
     <row r="182" spans="2:14" x14ac:dyDescent="0.25">
@@ -31063,7 +31063,7 @@
       </c>
       <c r="D184" s="376">
         <f>'Crude refineries'!AC6</f>
-        <v>0.95198971146726152</v>
+        <v>0.96412108310809064</v>
       </c>
       <c r="J184" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31078,7 +31078,7 @@
       </c>
       <c r="N184" s="301">
         <f>D184</f>
-        <v>0.95198971146726152</v>
+        <v>0.96412108310809064</v>
       </c>
     </row>
     <row r="185" spans="2:14" x14ac:dyDescent="0.25">
@@ -31124,7 +31124,7 @@
       </c>
       <c r="D187" s="375">
         <f>'Crude refineries'!$AF$14</f>
-        <v>0.35276939364868132</v>
+        <v>0.34833055635651694</v>
       </c>
       <c r="J187" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31139,7 +31139,7 @@
       </c>
       <c r="N187" s="301">
         <f t="shared" si="19"/>
-        <v>0.35276939364868132</v>
+        <v>0.34833055635651694</v>
       </c>
     </row>
     <row r="188" spans="2:14" x14ac:dyDescent="0.25">
@@ -31148,7 +31148,7 @@
       </c>
       <c r="D188" s="375">
         <f>'Crude refineries'!$AF$15</f>
-        <v>0.20197781416846072</v>
+        <v>0.19943636167892398</v>
       </c>
       <c r="J188" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31163,7 +31163,7 @@
       </c>
       <c r="N188" s="301">
         <f t="shared" si="19"/>
-        <v>0.20197781416846072</v>
+        <v>0.19943636167892398</v>
       </c>
     </row>
     <row r="189" spans="2:14" x14ac:dyDescent="0.25">
@@ -31172,7 +31172,7 @@
       </c>
       <c r="D189" s="375">
         <f>'Crude refineries'!$AF$17</f>
-        <v>0.12524521696188154</v>
+        <v>0.12366927769468629</v>
       </c>
       <c r="J189" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31187,7 +31187,7 @@
       </c>
       <c r="N189" s="301">
         <f t="shared" si="19"/>
-        <v>0.12524521696188154</v>
+        <v>0.12366927769468629</v>
       </c>
     </row>
     <row r="190" spans="2:14" x14ac:dyDescent="0.25">
@@ -31196,7 +31196,7 @@
       </c>
       <c r="D190" s="375">
         <f>'Crude refineries'!$AF$18</f>
-        <v>0</v>
+        <v>1.2582829950902787E-2</v>
       </c>
       <c r="J190" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31211,7 +31211,7 @@
       </c>
       <c r="N190" s="301">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.2582829950902787E-2</v>
       </c>
     </row>
     <row r="191" spans="2:14" x14ac:dyDescent="0.25">
@@ -31220,7 +31220,7 @@
       </c>
       <c r="D191" s="375">
         <f>SUM('Crude refineries'!$AF$20:$AF$23)</f>
-        <v>0.3002204613879127</v>
+        <v>0.29644283837448704</v>
       </c>
       <c r="J191" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31235,7 +31235,7 @@
       </c>
       <c r="N191" s="301">
         <f t="shared" si="19"/>
-        <v>0.3002204613879127</v>
+        <v>0.29644283837448704</v>
       </c>
     </row>
     <row r="192" spans="2:14" x14ac:dyDescent="0.25">
@@ -31244,7 +31244,7 @@
       </c>
       <c r="D192" s="375">
         <f>1-SUM(D186:D191)</f>
-        <v>1.9787113833063752E-2</v>
+        <v>1.9538135944482948E-2</v>
       </c>
       <c r="J192" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31259,7 +31259,7 @@
       </c>
       <c r="N192" s="301">
         <f t="shared" si="19"/>
-        <v>1.9787113833063752E-2</v>
+        <v>1.9538135944482948E-2</v>
       </c>
     </row>
     <row r="193" spans="2:20" x14ac:dyDescent="0.25">
@@ -31271,7 +31271,7 @@
       </c>
       <c r="D193" s="377">
         <f>'Crude refineries'!AC26</f>
-        <v>173597.75998964717</v>
+        <v>175809.94665204713</v>
       </c>
       <c r="J193" s="252" t="str">
         <f t="shared" si="17"/>
@@ -31340,7 +31340,7 @@
       </c>
       <c r="N195" s="299">
         <f>D193/D194/1000</f>
-        <v>190.08954718866366</v>
+        <v>192.51189158399163</v>
       </c>
     </row>
     <row r="196" spans="2:20" x14ac:dyDescent="0.25">
@@ -31375,7 +31375,7 @@
       </c>
       <c r="N197" s="295">
         <f>N196+$D$107/N184</f>
-        <v>218.94165930864898</v>
+        <v>216.53609229098166</v>
       </c>
     </row>
     <row r="198" spans="2:20" x14ac:dyDescent="0.25">
@@ -31394,7 +31394,7 @@
       </c>
       <c r="N198" s="295">
         <f>N196+$D$108/N184</f>
-        <v>282.66783821153194</v>
+        <v>279.46041552130885</v>
       </c>
     </row>
     <row r="200" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31487,7 +31487,7 @@
       </c>
       <c r="N204" s="481">
         <f>N181</f>
-        <v>4.5130780547547305E-3</v>
+        <v>4.4562907610366017E-3</v>
       </c>
       <c r="R204" t="s">
         <v>556</v>
@@ -34393,7 +34393,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE28" sqref="AE28"/>
+      <selection pane="topRight" activeCell="AC17" sqref="AC17:AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34451,26 +34451,26 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="96" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="496" t="s">
+      <c r="C2" s="486" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="497"/>
-      <c r="E2" s="497"/>
-      <c r="F2" s="498" t="s">
+      <c r="D2" s="487"/>
+      <c r="E2" s="487"/>
+      <c r="F2" s="488" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="499"/>
-      <c r="H2" s="500"/>
-      <c r="I2" s="498" t="s">
+      <c r="G2" s="489"/>
+      <c r="H2" s="490"/>
+      <c r="I2" s="488" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="499"/>
-      <c r="K2" s="500"/>
-      <c r="L2" s="498" t="s">
+      <c r="J2" s="489"/>
+      <c r="K2" s="490"/>
+      <c r="L2" s="488" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="499"/>
-      <c r="N2" s="500"/>
+      <c r="M2" s="489"/>
+      <c r="N2" s="490"/>
       <c r="O2" s="97"/>
       <c r="P2" s="13"/>
       <c r="AA2" s="96" t="s">
@@ -34678,7 +34678,7 @@
       </c>
       <c r="AC6" s="92">
         <f>AC26/AC5</f>
-        <v>0.95198971146726152</v>
+        <v>0.96412108310809064</v>
       </c>
       <c r="AD6" s="92">
         <f>AD26/AD5</f>
@@ -34743,10 +34743,10 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="485" t="s">
+      <c r="A9" s="491" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="486"/>
+      <c r="B9" s="492"/>
       <c r="C9" s="49"/>
       <c r="D9" s="44">
         <f>D5/$O$5</f>
@@ -34771,49 +34771,49 @@
       <c r="O9" s="7">
         <v>788</v>
       </c>
-      <c r="Q9" s="491" t="s">
+      <c r="Q9" s="497" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="493" t="s">
+      <c r="S9" s="499" t="s">
         <v>83</v>
       </c>
-      <c r="V9" s="489" t="s">
+      <c r="V9" s="495" t="s">
         <v>881</v>
       </c>
-      <c r="W9" s="489" t="s">
+      <c r="W9" s="495" t="s">
         <v>882</v>
       </c>
-      <c r="X9" s="489" t="s">
+      <c r="X9" s="495" t="s">
         <v>82</v>
       </c>
-      <c r="Y9" s="489" t="s">
+      <c r="Y9" s="495" t="s">
         <v>883</v>
       </c>
-      <c r="Z9" s="489" t="s">
+      <c r="Z9" s="495" t="s">
         <v>884</v>
       </c>
-      <c r="AA9" s="489" t="s">
+      <c r="AA9" s="495" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="489" t="s">
+      <c r="AB9" s="495" t="s">
         <v>885</v>
       </c>
-      <c r="AC9" s="489" t="s">
+      <c r="AC9" s="495" t="s">
         <v>886</v>
       </c>
-      <c r="AD9" s="489" t="s">
+      <c r="AD9" s="495" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="489" t="s">
+      <c r="AE9" s="495" t="s">
         <v>887</v>
       </c>
-      <c r="AF9" s="489" t="s">
+      <c r="AF9" s="495" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="487"/>
-      <c r="B10" s="488"/>
+      <c r="A10" s="493"/>
+      <c r="B10" s="494"/>
       <c r="C10" s="49"/>
       <c r="D10" s="9">
         <f>D9*788</f>
@@ -34839,25 +34839,25 @@
         <f>O9-G10</f>
         <v>422.2729198252656</v>
       </c>
-      <c r="Q10" s="492"/>
+      <c r="Q10" s="498"/>
       <c r="R10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="S10" s="494"/>
+      <c r="S10" s="500"/>
       <c r="U10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="V10" s="490"/>
-      <c r="W10" s="490"/>
-      <c r="X10" s="490"/>
-      <c r="Y10" s="490"/>
-      <c r="Z10" s="490"/>
-      <c r="AA10" s="490"/>
-      <c r="AB10" s="490"/>
-      <c r="AC10" s="490"/>
-      <c r="AD10" s="490"/>
-      <c r="AE10" s="490"/>
-      <c r="AF10" s="490"/>
+      <c r="V10" s="496"/>
+      <c r="W10" s="496"/>
+      <c r="X10" s="496"/>
+      <c r="Y10" s="496"/>
+      <c r="Z10" s="496"/>
+      <c r="AA10" s="496"/>
+      <c r="AB10" s="496"/>
+      <c r="AC10" s="496"/>
+      <c r="AD10" s="496"/>
+      <c r="AE10" s="496"/>
+      <c r="AF10" s="496"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
@@ -35072,7 +35072,7 @@
       </c>
       <c r="AF12" s="51">
         <f t="shared" ref="AF12:AF25" si="14">AC12/$AC$26</f>
-        <v>1.0274852538341359E-2</v>
+        <v>1.0145565816080809E-2</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
@@ -35173,7 +35173,7 @@
       </c>
       <c r="AF13" s="51">
         <f t="shared" si="14"/>
-        <v>8.898113450842458E-3</v>
+        <v>8.7861500024066681E-3</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
@@ -35285,7 +35285,7 @@
       </c>
       <c r="AF14" s="51">
         <f t="shared" si="14"/>
-        <v>0.35276939364868132</v>
+        <v>0.34833055635651694</v>
       </c>
       <c r="AG14" s="73">
         <f>AD14+AB14</f>
@@ -35404,7 +35404,7 @@
       </c>
       <c r="AF15" s="51">
         <f t="shared" si="14"/>
-        <v>0.20197781416846072</v>
+        <v>0.19943636167892398</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
@@ -35610,7 +35610,7 @@
       </c>
       <c r="AF17" s="51">
         <f t="shared" si="14"/>
-        <v>0.12524521696188154</v>
+        <v>0.12366927769468629</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
@@ -35707,7 +35707,10 @@
         <f t="shared" si="13"/>
         <v>10901.40062</v>
       </c>
-      <c r="AC18" s="50"/>
+      <c r="AC18" s="50">
+        <f t="shared" si="13"/>
+        <v>2212.1866623999999</v>
+      </c>
       <c r="AD18" s="50">
         <f t="shared" si="7"/>
         <v>539.60618239120879</v>
@@ -35718,7 +35721,7 @@
       </c>
       <c r="AF18" s="51">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.2582829950902787E-2</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="26.25" x14ac:dyDescent="0.25">
@@ -36028,7 +36031,7 @@
       </c>
       <c r="AF21" s="51">
         <f t="shared" si="14"/>
-        <v>4.9268462856375962E-2</v>
+        <v>4.8648526166311823E-2</v>
       </c>
       <c r="AG21" s="73">
         <f>SUM(AB21:AB23)+SUM(AD21:AD23)</f>
@@ -36146,7 +36149,7 @@
       </c>
       <c r="AF22" s="51">
         <f t="shared" si="14"/>
-        <v>2.620034210275091E-2</v>
+        <v>2.5870667653416522E-2</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.2">
@@ -36256,7 +36259,7 @@
       </c>
       <c r="AF23" s="51">
         <f t="shared" si="14"/>
-        <v>0.22475165642878581</v>
+        <v>0.22192364455475871</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
@@ -36356,7 +36359,7 @@
       </c>
       <c r="AF24" s="51">
         <f t="shared" si="14"/>
-        <v>6.1414784387977227E-4</v>
+        <v>6.0642012599551956E-4</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="15" x14ac:dyDescent="0.25">
@@ -36522,7 +36525,7 @@
       </c>
       <c r="AC26" s="45">
         <f>SUM(AC11:AC25)</f>
-        <v>173597.75998964717</v>
+        <v>175809.94665204713</v>
       </c>
       <c r="AD26" s="45">
         <f>SUM(AD11:AD25)</f>
@@ -37346,11 +37349,11 @@
       <c r="J62" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="495" t="s">
+      <c r="K62" s="485" t="s">
         <v>26</v>
       </c>
-      <c r="L62" s="495"/>
-      <c r="M62" s="495"/>
+      <c r="L62" s="485"/>
+      <c r="M62" s="485"/>
       <c r="N62"/>
     </row>
     <row r="63" spans="3:22" ht="15" x14ac:dyDescent="0.25">
@@ -37608,11 +37611,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AC9:AC10"/>
@@ -37627,6 +37625,11 @@
     <mergeCell ref="AB9:AB10"/>
     <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="W9:W10"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40295,7 +40298,7 @@
         <v>190</v>
       </c>
       <c r="G2" s="509"/>
-      <c r="H2" s="500"/>
+      <c r="H2" s="490"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -40537,7 +40540,7 @@
       <c r="G14" s="88"/>
       <c r="H14" s="154"/>
       <c r="I14" s="153"/>
-      <c r="J14" s="494"/>
+      <c r="J14" s="500"/>
       <c r="K14" s="152" t="s">
         <v>79</v>
       </c>
@@ -44425,27 +44428,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="521" t="s">
+      <c r="A1" s="513" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="516"/>
-      <c r="C1" s="516"/>
-      <c r="D1" s="516"/>
-      <c r="E1" s="516"/>
-      <c r="F1" s="516"/>
-      <c r="G1" s="516"/>
-      <c r="H1" s="516"/>
-      <c r="I1" s="516"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
       <c r="J1" s="216" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="522" t="s">
+      <c r="A2" s="515" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
+      <c r="B2" s="515"/>
+      <c r="C2" s="515"/>
       <c r="D2" s="259">
         <v>2019</v>
       </c>
@@ -44482,16 +44485,16 @@
       <c r="U2" s="252"/>
     </row>
     <row r="3" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="523" t="s">
+      <c r="A3" s="516" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="523"/>
+      <c r="B3" s="516"/>
       <c r="C3" s="254"/>
       <c r="D3" s="255"/>
       <c r="E3" s="254"/>
       <c r="F3" s="254"/>
       <c r="G3" s="253"/>
-      <c r="H3" s="524" t="s">
+      <c r="H3" s="517" t="s">
         <v>373</v>
       </c>
       <c r="Q3"/>
@@ -44501,10 +44504,10 @@
       <c r="U3" s="252"/>
     </row>
     <row r="4" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="527" t="s">
+      <c r="A4" s="520" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="527"/>
+      <c r="B4" s="520"/>
       <c r="C4" s="241">
         <v>1</v>
       </c>
@@ -44520,7 +44523,7 @@
       <c r="G4" s="221">
         <v>18806</v>
       </c>
-      <c r="H4" s="525"/>
+      <c r="H4" s="518"/>
       <c r="J4" s="216">
         <f>D4/F4</f>
         <v>0.99859246427024684</v>
@@ -44538,10 +44541,10 @@
       <c r="T4" s="252"/>
     </row>
     <row r="5" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="513" t="s">
+      <c r="A5" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="513"/>
+      <c r="B5" s="521"/>
       <c r="C5" s="239"/>
       <c r="D5" s="231">
         <v>6736</v>
@@ -44555,13 +44558,13 @@
       <c r="G5" s="221">
         <v>7019</v>
       </c>
-      <c r="H5" s="525"/>
+      <c r="H5" s="518"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="513" t="s">
+      <c r="A6" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="513"/>
+      <c r="B6" s="521"/>
       <c r="C6" s="239"/>
       <c r="D6" s="231">
         <v>1467</v>
@@ -44575,13 +44578,13 @@
       <c r="G6" s="221">
         <v>1461</v>
       </c>
-      <c r="H6" s="525"/>
+      <c r="H6" s="518"/>
     </row>
     <row r="7" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="513" t="s">
+      <c r="A7" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="513"/>
+      <c r="B7" s="521"/>
       <c r="C7" s="239"/>
       <c r="D7" s="231">
         <v>3209</v>
@@ -44595,13 +44598,13 @@
       <c r="G7" s="221">
         <v>3331</v>
       </c>
-      <c r="H7" s="525"/>
+      <c r="H7" s="518"/>
     </row>
     <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="513" t="s">
+      <c r="A8" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B8" s="513"/>
+      <c r="B8" s="521"/>
       <c r="C8" s="239"/>
       <c r="D8" s="231">
         <v>4271</v>
@@ -44615,13 +44618,13 @@
       <c r="G8" s="221">
         <v>4067</v>
       </c>
-      <c r="H8" s="525"/>
+      <c r="H8" s="518"/>
     </row>
     <row r="9" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="513" t="s">
+      <c r="A9" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="513"/>
+      <c r="B9" s="521"/>
       <c r="C9" s="239"/>
       <c r="D9" s="231">
         <v>1277</v>
@@ -44635,13 +44638,13 @@
       <c r="G9" s="221">
         <v>1309</v>
       </c>
-      <c r="H9" s="525"/>
+      <c r="H9" s="518"/>
     </row>
     <row r="10" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="513" t="s">
+      <c r="A10" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="513"/>
+      <c r="B10" s="521"/>
       <c r="C10" s="239"/>
       <c r="D10" s="233">
         <v>688</v>
@@ -44655,13 +44658,13 @@
       <c r="G10" s="218">
         <v>793</v>
       </c>
-      <c r="H10" s="525"/>
+      <c r="H10" s="518"/>
     </row>
     <row r="11" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="513" t="s">
+      <c r="A11" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="513"/>
+      <c r="B11" s="521"/>
       <c r="C11" s="239"/>
       <c r="D11" s="233">
         <v>53</v>
@@ -44675,14 +44678,14 @@
       <c r="G11" s="218">
         <v>62</v>
       </c>
-      <c r="H11" s="525"/>
+      <c r="H11" s="518"/>
     </row>
     <row r="12" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="514" t="s">
+      <c r="A12" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B12" s="514"/>
-      <c r="C12" s="514"/>
+      <c r="B12" s="522"/>
+      <c r="C12" s="522"/>
       <c r="D12" s="251">
         <v>745</v>
       </c>
@@ -44695,14 +44698,14 @@
       <c r="G12" s="249">
         <v>763</v>
       </c>
-      <c r="H12" s="526"/>
+      <c r="H12" s="519"/>
       <c r="V12" s="243"/>
     </row>
     <row r="13" spans="1:22" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="520" t="s">
+      <c r="A13" s="523" t="s">
         <v>396</v>
       </c>
-      <c r="B13" s="520"/>
+      <c r="B13" s="523"/>
       <c r="C13" s="248">
         <v>2</v>
       </c>
@@ -44714,10 +44717,10 @@
       <c r="V13" s="243"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="516" t="s">
+      <c r="A14" s="514" t="s">
         <v>395</v>
       </c>
-      <c r="B14" s="516"/>
+      <c r="B14" s="514"/>
       <c r="C14" s="239"/>
       <c r="D14" s="231">
         <v>105.04</v>
@@ -44752,10 +44755,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="513" t="s">
+      <c r="A15" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="513"/>
+      <c r="B15" s="521"/>
       <c r="C15" s="239"/>
       <c r="D15" s="231">
         <v>96.16</v>
@@ -44788,10 +44791,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="513" t="s">
+      <c r="A16" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="513"/>
+      <c r="B16" s="521"/>
       <c r="C16" s="239"/>
       <c r="D16" s="231">
         <v>5.34</v>
@@ -44824,10 +44827,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="513" t="s">
+      <c r="A17" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B17" s="513"/>
+      <c r="B17" s="521"/>
       <c r="C17" s="239"/>
       <c r="D17" s="231">
         <v>3.49</v>
@@ -44860,10 +44863,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="513" t="s">
+      <c r="A18" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B18" s="513"/>
+      <c r="B18" s="521"/>
       <c r="C18" s="239"/>
       <c r="D18" s="242">
         <v>0</v>
@@ -44896,10 +44899,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="513" t="s">
+      <c r="A19" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="513"/>
+      <c r="B19" s="521"/>
       <c r="C19" s="239"/>
       <c r="D19" s="231">
         <v>0</v>
@@ -44932,10 +44935,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="513" t="s">
+      <c r="A20" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B20" s="513"/>
+      <c r="B20" s="521"/>
       <c r="C20" s="239"/>
       <c r="D20" s="231">
         <v>0.04</v>
@@ -44968,10 +44971,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="513" t="s">
+      <c r="A21" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B21" s="513"/>
+      <c r="B21" s="521"/>
       <c r="C21" s="239"/>
       <c r="D21" s="231">
         <v>0</v>
@@ -45004,11 +45007,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="513" t="s">
+      <c r="A22" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B22" s="513"/>
-      <c r="C22" s="513"/>
+      <c r="B22" s="521"/>
+      <c r="C22" s="521"/>
       <c r="D22" s="231">
         <v>0.01</v>
       </c>
@@ -45040,10 +45043,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="516" t="s">
+      <c r="A23" s="514" t="s">
         <v>394</v>
       </c>
-      <c r="B23" s="516"/>
+      <c r="B23" s="514"/>
       <c r="C23" s="239"/>
       <c r="D23" s="231">
         <v>1.64</v>
@@ -45078,10 +45081,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="513" t="s">
+      <c r="A24" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B24" s="513"/>
+      <c r="B24" s="521"/>
       <c r="C24" s="239"/>
       <c r="D24" s="231">
         <v>0.9</v>
@@ -45114,10 +45117,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="513" t="s">
+      <c r="A25" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="513"/>
+      <c r="B25" s="521"/>
       <c r="C25" s="239"/>
       <c r="D25" s="231">
         <v>0.73</v>
@@ -45150,10 +45153,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="513" t="s">
+      <c r="A26" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B26" s="513"/>
+      <c r="B26" s="521"/>
       <c r="C26" s="239"/>
       <c r="D26" s="231">
         <v>0</v>
@@ -45186,10 +45189,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="513" t="s">
+      <c r="A27" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B27" s="513"/>
+      <c r="B27" s="521"/>
       <c r="C27" s="239"/>
       <c r="D27" s="231">
         <v>0</v>
@@ -45222,10 +45225,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="513" t="s">
+      <c r="A28" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="513"/>
+      <c r="B28" s="521"/>
       <c r="C28" s="239"/>
       <c r="D28" s="231">
         <v>0</v>
@@ -45258,10 +45261,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="513" t="s">
+      <c r="A29" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B29" s="513"/>
+      <c r="B29" s="521"/>
       <c r="C29" s="239"/>
       <c r="D29" s="231">
         <v>0.01</v>
@@ -45294,10 +45297,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="513" t="s">
+      <c r="A30" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B30" s="513"/>
+      <c r="B30" s="521"/>
       <c r="C30" s="239"/>
       <c r="D30" s="231">
         <v>0</v>
@@ -45330,11 +45333,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="513" t="s">
+      <c r="A31" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B31" s="513"/>
-      <c r="C31" s="513"/>
+      <c r="B31" s="521"/>
+      <c r="C31" s="521"/>
       <c r="D31" s="231">
         <v>0</v>
       </c>
@@ -45366,10 +45369,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="516" t="s">
+      <c r="A32" s="514" t="s">
         <v>393</v>
       </c>
-      <c r="B32" s="516"/>
+      <c r="B32" s="514"/>
       <c r="C32" s="239"/>
       <c r="D32" s="231">
         <v>56004</v>
@@ -45404,10 +45407,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="513" t="s">
+      <c r="A33" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B33" s="513"/>
+      <c r="B33" s="521"/>
       <c r="C33" s="239"/>
       <c r="D33" s="231">
         <v>48418</v>
@@ -45446,10 +45449,10 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="513" t="s">
+      <c r="A34" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="513"/>
+      <c r="B34" s="521"/>
       <c r="C34" s="239"/>
       <c r="D34" s="231">
         <v>4557</v>
@@ -45482,10 +45485,10 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="513" t="s">
+      <c r="A35" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B35" s="513"/>
+      <c r="B35" s="521"/>
       <c r="C35" s="239"/>
       <c r="D35" s="233">
         <v>16</v>
@@ -45518,10 +45521,10 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="513" t="s">
+      <c r="A36" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B36" s="513"/>
+      <c r="B36" s="521"/>
       <c r="C36" s="239"/>
       <c r="D36" s="233">
         <v>932</v>
@@ -45554,10 +45557,10 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="513" t="s">
+      <c r="A37" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B37" s="513"/>
+      <c r="B37" s="521"/>
       <c r="C37" s="239"/>
       <c r="D37" s="233">
         <v>610</v>
@@ -45590,10 +45593,10 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="513" t="s">
+      <c r="A38" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="513"/>
+      <c r="B38" s="521"/>
       <c r="C38" s="239"/>
       <c r="D38" s="231">
         <v>1163</v>
@@ -45626,10 +45629,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="513" t="s">
+      <c r="A39" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B39" s="513"/>
+      <c r="B39" s="521"/>
       <c r="C39" s="239"/>
       <c r="D39" s="233">
         <v>261</v>
@@ -45662,11 +45665,11 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="513" t="s">
+      <c r="A40" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B40" s="513"/>
-      <c r="C40" s="513"/>
+      <c r="B40" s="521"/>
+      <c r="C40" s="521"/>
       <c r="D40" s="233">
         <v>47</v>
       </c>
@@ -45698,10 +45701,10 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="516" t="s">
+      <c r="A41" s="514" t="s">
         <v>391</v>
       </c>
-      <c r="B41" s="516"/>
+      <c r="B41" s="514"/>
       <c r="C41" s="241">
         <v>3</v>
       </c>
@@ -45722,10 +45725,10 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="513" t="s">
+      <c r="A42" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B42" s="513"/>
+      <c r="B42" s="521"/>
       <c r="C42" s="239"/>
       <c r="D42" s="231">
         <v>5596</v>
@@ -45761,10 +45764,10 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="513" t="s">
+      <c r="A43" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="513"/>
+      <c r="B43" s="521"/>
       <c r="C43" s="239"/>
       <c r="D43" s="233">
         <v>400</v>
@@ -45800,10 +45803,10 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="513" t="s">
+      <c r="A44" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B44" s="513"/>
+      <c r="B44" s="521"/>
       <c r="C44" s="239"/>
       <c r="D44" s="233">
         <v>726</v>
@@ -45839,10 +45842,10 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="513" t="s">
+      <c r="A45" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="513"/>
+      <c r="B45" s="521"/>
       <c r="C45" s="239"/>
       <c r="D45" s="233">
         <v>289</v>
@@ -45878,10 +45881,10 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="513" t="s">
+      <c r="A46" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B46" s="513"/>
+      <c r="B46" s="521"/>
       <c r="C46" s="239"/>
       <c r="D46" s="233">
         <v>108</v>
@@ -45898,10 +45901,10 @@
       <c r="H46" s="230"/>
     </row>
     <row r="47" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="513" t="s">
+      <c r="A47" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="513"/>
+      <c r="B47" s="521"/>
       <c r="C47" s="239"/>
       <c r="D47" s="233">
         <v>498</v>
@@ -45918,10 +45921,10 @@
       <c r="H47" s="230"/>
     </row>
     <row r="48" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="513" t="s">
+      <c r="A48" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="513"/>
+      <c r="B48" s="521"/>
       <c r="C48" s="239"/>
       <c r="D48" s="231">
         <v>0</v>
@@ -45938,11 +45941,11 @@
       <c r="H48" s="230"/>
     </row>
     <row r="49" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="513" t="s">
+      <c r="A49" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="513"/>
-      <c r="C49" s="513"/>
+      <c r="B49" s="521"/>
+      <c r="C49" s="521"/>
       <c r="D49" s="233">
         <v>36</v>
       </c>
@@ -45958,10 +45961,10 @@
       <c r="H49" s="230"/>
     </row>
     <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="516" t="s">
+      <c r="A50" s="514" t="s">
         <v>390</v>
       </c>
-      <c r="B50" s="516"/>
+      <c r="B50" s="514"/>
       <c r="C50" s="241">
         <v>4</v>
       </c>
@@ -45982,10 +45985,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="513" t="s">
+      <c r="A51" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B51" s="513"/>
+      <c r="B51" s="521"/>
       <c r="C51" s="239"/>
       <c r="D51" s="231">
         <v>0</v>
@@ -46002,10 +46005,10 @@
       <c r="H51" s="230"/>
     </row>
     <row r="52" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="513" t="s">
+      <c r="A52" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B52" s="513"/>
+      <c r="B52" s="521"/>
       <c r="C52" s="239"/>
       <c r="D52" s="231">
         <v>0</v>
@@ -46022,10 +46025,10 @@
       <c r="H52" s="230"/>
     </row>
     <row r="53" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="513" t="s">
+      <c r="A53" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B53" s="513"/>
+      <c r="B53" s="521"/>
       <c r="C53" s="239"/>
       <c r="D53" s="231">
         <v>0</v>
@@ -46042,10 +46045,10 @@
       <c r="H53" s="230"/>
     </row>
     <row r="54" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="513" t="s">
+      <c r="A54" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B54" s="513"/>
+      <c r="B54" s="521"/>
       <c r="C54" s="239"/>
       <c r="D54" s="231">
         <v>0</v>
@@ -46062,10 +46065,10 @@
       <c r="H54" s="230"/>
     </row>
     <row r="55" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="513" t="s">
+      <c r="A55" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B55" s="513"/>
+      <c r="B55" s="521"/>
       <c r="C55" s="239"/>
       <c r="D55" s="231">
         <v>0</v>
@@ -46082,10 +46085,10 @@
       <c r="H55" s="230"/>
     </row>
     <row r="56" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="513" t="s">
+      <c r="A56" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B56" s="513"/>
+      <c r="B56" s="521"/>
       <c r="C56" s="239"/>
       <c r="D56" s="231">
         <v>0</v>
@@ -46102,10 +46105,10 @@
       <c r="H56" s="230"/>
     </row>
     <row r="57" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="513" t="s">
+      <c r="A57" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="513"/>
+      <c r="B57" s="521"/>
       <c r="C57" s="239"/>
       <c r="D57" s="231">
         <v>0.05</v>
@@ -46122,11 +46125,11 @@
       <c r="H57" s="230"/>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="514" t="s">
+      <c r="A58" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B58" s="514"/>
-      <c r="C58" s="514"/>
+      <c r="B58" s="522"/>
+      <c r="C58" s="522"/>
       <c r="D58" s="229">
         <v>0</v>
       </c>
@@ -46142,46 +46145,46 @@
       <c r="H58" s="238"/>
     </row>
     <row r="59" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="516"/>
-      <c r="B59" s="516"/>
-      <c r="C59" s="516"/>
-      <c r="D59" s="516"/>
-      <c r="E59" s="516"/>
-      <c r="F59" s="516"/>
-      <c r="G59" s="516"/>
-      <c r="H59" s="516"/>
-      <c r="I59" s="516"/>
+      <c r="A59" s="514"/>
+      <c r="B59" s="514"/>
+      <c r="C59" s="514"/>
+      <c r="D59" s="514"/>
+      <c r="E59" s="514"/>
+      <c r="F59" s="514"/>
+      <c r="G59" s="514"/>
+      <c r="H59" s="514"/>
+      <c r="I59" s="514"/>
     </row>
     <row r="60" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="516"/>
-      <c r="B60" s="516"/>
-      <c r="C60" s="516"/>
-      <c r="D60" s="516"/>
-      <c r="E60" s="516"/>
-      <c r="F60" s="516"/>
-      <c r="G60" s="516"/>
-      <c r="H60" s="516"/>
-      <c r="I60" s="516"/>
+      <c r="A60" s="514"/>
+      <c r="B60" s="514"/>
+      <c r="C60" s="514"/>
+      <c r="D60" s="514"/>
+      <c r="E60" s="514"/>
+      <c r="F60" s="514"/>
+      <c r="G60" s="514"/>
+      <c r="H60" s="514"/>
+      <c r="I60" s="514"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="519" t="s">
+      <c r="A61" s="524" t="s">
         <v>388</v>
       </c>
-      <c r="B61" s="519"/>
-      <c r="C61" s="519"/>
-      <c r="D61" s="519"/>
-      <c r="E61" s="519"/>
-      <c r="F61" s="519"/>
-      <c r="G61" s="519"/>
-      <c r="H61" s="519"/>
-      <c r="I61" s="519"/>
+      <c r="B61" s="524"/>
+      <c r="C61" s="524"/>
+      <c r="D61" s="524"/>
+      <c r="E61" s="524"/>
+      <c r="F61" s="524"/>
+      <c r="G61" s="524"/>
+      <c r="H61" s="524"/>
+      <c r="I61" s="524"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="517" t="s">
+      <c r="A62" s="525" t="s">
         <v>345</v>
       </c>
-      <c r="B62" s="517"/>
-      <c r="C62" s="517"/>
+      <c r="B62" s="525"/>
+      <c r="C62" s="525"/>
       <c r="D62" s="225">
         <v>2019</v>
       </c>
@@ -46199,11 +46202,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="518" t="s">
+      <c r="A63" s="526" t="s">
         <v>344</v>
       </c>
-      <c r="B63" s="518"/>
-      <c r="C63" s="518"/>
+      <c r="B63" s="526"/>
+      <c r="C63" s="526"/>
       <c r="D63" s="220" t="s">
         <v>386</v>
       </c>
@@ -46221,11 +46224,11 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="513" t="s">
+      <c r="A64" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="513"/>
-      <c r="C64" s="513"/>
+      <c r="B64" s="521"/>
+      <c r="C64" s="521"/>
       <c r="D64" s="231" t="s">
         <v>382</v>
       </c>
@@ -46241,11 +46244,11 @@
       <c r="H64" s="230"/>
     </row>
     <row r="65" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="513" t="s">
+      <c r="A65" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B65" s="513"/>
-      <c r="C65" s="513"/>
+      <c r="B65" s="521"/>
+      <c r="C65" s="521"/>
       <c r="D65" s="231" t="s">
         <v>380</v>
       </c>
@@ -46261,11 +46264,11 @@
       <c r="H65" s="230"/>
     </row>
     <row r="66" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="513" t="s">
+      <c r="A66" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B66" s="513"/>
-      <c r="C66" s="513"/>
+      <c r="B66" s="521"/>
+      <c r="C66" s="521"/>
       <c r="D66" s="233">
         <v>822</v>
       </c>
@@ -46281,11 +46284,11 @@
       <c r="H66" s="230"/>
     </row>
     <row r="67" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="513" t="s">
+      <c r="A67" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B67" s="513"/>
-      <c r="C67" s="513"/>
+      <c r="B67" s="521"/>
+      <c r="C67" s="521"/>
       <c r="D67" s="231" t="s">
         <v>379</v>
       </c>
@@ -46301,11 +46304,11 @@
       <c r="H67" s="230"/>
     </row>
     <row r="68" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="513" t="s">
+      <c r="A68" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="513"/>
-      <c r="C68" s="513"/>
+      <c r="B68" s="521"/>
+      <c r="C68" s="521"/>
       <c r="D68" s="233">
         <v>717</v>
       </c>
@@ -46321,11 +46324,11 @@
       <c r="H68" s="230"/>
     </row>
     <row r="69" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="513" t="s">
+      <c r="A69" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="513"/>
-      <c r="C69" s="513"/>
+      <c r="B69" s="521"/>
+      <c r="C69" s="521"/>
       <c r="D69" s="231" t="s">
         <v>378</v>
       </c>
@@ -46341,11 +46344,11 @@
       <c r="H69" s="230"/>
     </row>
     <row r="70" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="513" t="s">
+      <c r="A70" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B70" s="513"/>
-      <c r="C70" s="513"/>
+      <c r="B70" s="521"/>
+      <c r="C70" s="521"/>
       <c r="D70" s="233">
         <v>261</v>
       </c>
@@ -46361,11 +46364,11 @@
       <c r="H70" s="230"/>
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="513" t="s">
+      <c r="A71" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B71" s="513"/>
-      <c r="C71" s="513"/>
+      <c r="B71" s="521"/>
+      <c r="C71" s="521"/>
       <c r="D71" s="233">
         <v>83</v>
       </c>
@@ -46381,11 +46384,11 @@
       <c r="H71" s="230"/>
     </row>
     <row r="72" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="516" t="s">
+      <c r="A72" s="514" t="s">
         <v>377</v>
       </c>
-      <c r="B72" s="516"/>
-      <c r="C72" s="516"/>
+      <c r="B72" s="514"/>
+      <c r="C72" s="514"/>
       <c r="D72" s="231" t="s">
         <v>368</v>
       </c>
@@ -46403,11 +46406,11 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="513" t="s">
+      <c r="A73" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B73" s="513"/>
-      <c r="C73" s="513"/>
+      <c r="B73" s="521"/>
+      <c r="C73" s="521"/>
       <c r="D73" s="231" t="s">
         <v>372</v>
       </c>
@@ -46423,11 +46426,11 @@
       <c r="H73" s="230"/>
     </row>
     <row r="74" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="513" t="s">
+      <c r="A74" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B74" s="513"/>
-      <c r="C74" s="513"/>
+      <c r="B74" s="521"/>
+      <c r="C74" s="521"/>
       <c r="D74" s="231" t="s">
         <v>368</v>
       </c>
@@ -46443,11 +46446,11 @@
       <c r="H74" s="230"/>
     </row>
     <row r="75" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="513" t="s">
+      <c r="A75" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B75" s="513"/>
-      <c r="C75" s="513"/>
+      <c r="B75" s="521"/>
+      <c r="C75" s="521"/>
       <c r="D75" s="231" t="s">
         <v>348</v>
       </c>
@@ -46463,11 +46466,11 @@
       <c r="H75" s="230"/>
     </row>
     <row r="76" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="513" t="s">
+      <c r="A76" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B76" s="513"/>
-      <c r="C76" s="513"/>
+      <c r="B76" s="521"/>
+      <c r="C76" s="521"/>
       <c r="D76" s="231" t="s">
         <v>362</v>
       </c>
@@ -46483,11 +46486,11 @@
       <c r="H76" s="230"/>
     </row>
     <row r="77" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="513" t="s">
+      <c r="A77" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B77" s="513"/>
-      <c r="C77" s="513"/>
+      <c r="B77" s="521"/>
+      <c r="C77" s="521"/>
       <c r="D77" s="231" t="s">
         <v>361</v>
       </c>
@@ -46503,11 +46506,11 @@
       <c r="H77" s="230"/>
     </row>
     <row r="78" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="513" t="s">
+      <c r="A78" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B78" s="513"/>
-      <c r="C78" s="513"/>
+      <c r="B78" s="521"/>
+      <c r="C78" s="521"/>
       <c r="D78" s="231" t="s">
         <v>358</v>
       </c>
@@ -46523,11 +46526,11 @@
       <c r="H78" s="230"/>
     </row>
     <row r="79" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="513" t="s">
+      <c r="A79" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="513"/>
-      <c r="C79" s="513"/>
+      <c r="B79" s="521"/>
+      <c r="C79" s="521"/>
       <c r="D79" s="231" t="s">
         <v>354</v>
       </c>
@@ -46543,11 +46546,11 @@
       <c r="H79" s="230"/>
     </row>
     <row r="80" spans="1:8" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="514" t="s">
+      <c r="A80" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B80" s="514"/>
-      <c r="C80" s="514"/>
+      <c r="B80" s="522"/>
+      <c r="C80" s="522"/>
       <c r="D80" s="229" t="s">
         <v>349</v>
       </c>
@@ -46563,30 +46566,30 @@
       <c r="H80" s="226"/>
     </row>
     <row r="81" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="515" t="s">
+      <c r="A81" s="527" t="s">
         <v>347</v>
       </c>
-      <c r="B81" s="516"/>
-      <c r="C81" s="516"/>
-      <c r="D81" s="516"/>
-      <c r="E81" s="516"/>
-      <c r="F81" s="516"/>
-      <c r="G81" s="516"/>
-      <c r="H81" s="516"/>
-      <c r="I81" s="516"/>
+      <c r="B81" s="514"/>
+      <c r="C81" s="514"/>
+      <c r="D81" s="514"/>
+      <c r="E81" s="514"/>
+      <c r="F81" s="514"/>
+      <c r="G81" s="514"/>
+      <c r="H81" s="514"/>
+      <c r="I81" s="514"/>
     </row>
     <row r="82" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="516" t="s">
+      <c r="A82" s="514" t="s">
         <v>346</v>
       </c>
-      <c r="B82" s="516"/>
-      <c r="C82" s="516"/>
-      <c r="D82" s="516"/>
-      <c r="E82" s="516"/>
-      <c r="F82" s="516"/>
-      <c r="G82" s="516"/>
-      <c r="H82" s="516"/>
-      <c r="I82" s="516"/>
+      <c r="B82" s="514"/>
+      <c r="C82" s="514"/>
+      <c r="D82" s="514"/>
+      <c r="E82" s="514"/>
+      <c r="F82" s="514"/>
+      <c r="G82" s="514"/>
+      <c r="H82" s="514"/>
+      <c r="I82" s="514"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D83" s="216" t="str">
@@ -46607,11 +46610,11 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="517" t="s">
+      <c r="A85" s="525" t="s">
         <v>345</v>
       </c>
-      <c r="B85" s="517"/>
-      <c r="C85" s="517"/>
+      <c r="B85" s="525"/>
+      <c r="C85" s="525"/>
       <c r="D85" s="225">
         <v>2019</v>
       </c>
@@ -46638,11 +46641,11 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="518" t="s">
+      <c r="A86" s="526" t="s">
         <v>344</v>
       </c>
-      <c r="B86" s="518"/>
-      <c r="C86" s="518"/>
+      <c r="B86" s="526"/>
+      <c r="C86" s="526"/>
       <c r="D86" s="220">
         <f>D14*gwpch4+D23*gwpn2o+D32+D41+D50</f>
         <v>66558.41</v>
@@ -46680,11 +46683,11 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="513" t="s">
+      <c r="A87" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B87" s="513"/>
-      <c r="C87" s="513"/>
+      <c r="B87" s="521"/>
+      <c r="C87" s="521"/>
       <c r="D87" s="220">
         <f t="shared" ref="D87:D94" si="14">D15*gwpch4+D24*gwpn2o+D33+D42+D51</f>
         <v>56492.08</v>
@@ -46719,11 +46722,11 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="513" t="s">
+      <c r="A88" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B88" s="513"/>
-      <c r="C88" s="513"/>
+      <c r="B88" s="521"/>
+      <c r="C88" s="521"/>
       <c r="D88" s="220">
         <f t="shared" si="14"/>
         <v>5295.9</v>
@@ -46758,11 +46761,11 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="513" t="s">
+      <c r="A89" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B89" s="513"/>
-      <c r="C89" s="513"/>
+      <c r="B89" s="521"/>
+      <c r="C89" s="521"/>
       <c r="D89" s="220">
         <f t="shared" si="14"/>
         <v>822.27</v>
@@ -46797,11 +46800,11 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="513" t="s">
+      <c r="A90" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B90" s="513"/>
-      <c r="C90" s="513"/>
+      <c r="B90" s="521"/>
+      <c r="C90" s="521"/>
       <c r="D90" s="220">
         <f t="shared" si="14"/>
         <v>1221</v>
@@ -46836,11 +46839,11 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="513" t="s">
+      <c r="A91" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B91" s="513"/>
-      <c r="C91" s="513"/>
+      <c r="B91" s="521"/>
+      <c r="C91" s="521"/>
       <c r="D91" s="220">
         <f t="shared" si="14"/>
         <v>718</v>
@@ -46875,11 +46878,11 @@
       </c>
     </row>
     <row r="92" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="513" t="s">
+      <c r="A92" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B92" s="513"/>
-      <c r="C92" s="513"/>
+      <c r="B92" s="521"/>
+      <c r="C92" s="521"/>
       <c r="D92" s="220">
         <f t="shared" si="14"/>
         <v>1664.88</v>
@@ -46914,11 +46917,11 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="513" t="s">
+      <c r="A93" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B93" s="513"/>
-      <c r="C93" s="513"/>
+      <c r="B93" s="521"/>
+      <c r="C93" s="521"/>
       <c r="D93" s="220">
         <f t="shared" si="14"/>
         <v>261.05</v>
@@ -46953,11 +46956,11 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="513" t="s">
+      <c r="A94" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B94" s="513"/>
-      <c r="C94" s="513"/>
+      <c r="B94" s="521"/>
+      <c r="C94" s="521"/>
       <c r="D94" s="220">
         <f t="shared" si="14"/>
         <v>83.22999999999999</v>
@@ -47041,15 +47044,74 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:H12"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:B23"/>
@@ -47066,74 +47128,15 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A60:I60"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A81" r:id="rId1" display="http://www.sasol.com/" xr:uid="{94E57AF8-CF1E-4A4A-992A-3647A9F5048E}"/>

</xml_diff>

<commit_message>
Fixes on PTRA, REF and SUP (switched to Ref/high Oil Price)
</commit_message>
<xml_diff>
--- a/VT_REGION1_REF.xlsx
+++ b/VT_REGION1_REF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28CB25-0F2D-4918-81B1-F6AA3D53C8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6B2AD8-FF79-48ED-BD19-13BBB5610ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="-16290" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -9468,24 +9468,6 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9515,6 +9497,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9552,10 +9552,31 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9574,27 +9595,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -18763,11 +18763,11 @@
   </sheetPr>
   <dimension ref="A1:BH117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="M97" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="8" topLeftCell="F48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AD116" sqref="AD116"/>
+      <selection pane="bottomRight" activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22470,14 +22470,14 @@
       </c>
       <c r="F50" s="435">
         <f>SUMIF(RefineriesData!$J$16:$J$270,$B50&amp;F$4,RefineriesData!$N$16:$N$270)</f>
-        <v>1.4398895185724963</v>
+        <v>1.3713233510214249</v>
       </c>
       <c r="G50" s="436"/>
       <c r="H50" s="436"/>
       <c r="I50" s="482"/>
       <c r="J50" s="439">
         <f>IFERROR(zar.2010*SUMIF(RefineriesData!$J$13:$J$269,$B50&amp;J$4,RefineriesData!$N$13:$N$269),"")</f>
-        <v>35.527165339469441</v>
+        <v>55.422377929572328</v>
       </c>
       <c r="M50" s="466">
         <f>M40</f>
@@ -22489,7 +22489,7 @@
       </c>
       <c r="O50" s="439">
         <f>SUMIF(RefineriesData!$J$13:$J$267,$B50&amp;O$4,RefineriesData!$N$13:$N$267)</f>
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="P50" s="435">
         <f>SUMIF(RefineriesData!$J$16:$J$269,$B50&amp;P$4,RefineriesData!$N$16:$N$269)</f>
@@ -22497,7 +22497,7 @@
       </c>
       <c r="Q50" s="441">
         <f>IFERROR(SUMIF(RefineriesData!$J$13:$J$269,$B50&amp;Q$4,RefineriesData!$N$13:$N$269),"")</f>
-        <v>129.54169999999999</v>
+        <v>202.08505199999999</v>
       </c>
       <c r="R50" s="435">
         <v>-6</v>
@@ -23154,14 +23154,14 @@
       </c>
       <c r="F60" s="435">
         <f>F50</f>
-        <v>1.4398895185724963</v>
+        <v>1.3713233510214249</v>
       </c>
       <c r="G60" s="436"/>
       <c r="H60" s="436"/>
       <c r="I60" s="482"/>
       <c r="J60" s="440">
         <f>J50</f>
-        <v>35.527165339469441</v>
+        <v>55.422377929572328</v>
       </c>
       <c r="M60" s="466">
         <f>M40</f>
@@ -23173,7 +23173,7 @@
       </c>
       <c r="O60" s="439">
         <f>O50</f>
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="P60" s="435">
         <f>P50</f>
@@ -23181,7 +23181,7 @@
       </c>
       <c r="Q60" s="441">
         <f>Q50</f>
-        <v>129.54169999999999</v>
+        <v>202.08505199999999</v>
       </c>
       <c r="R60" s="435">
         <v>-6</v>
@@ -26550,8 +26550,8 @@
   </sheetPr>
   <dimension ref="A1:AH286"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="N267" sqref="N267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33568,8 +33568,8 @@
         <v>Main Fuel Efficiency</v>
       </c>
       <c r="N252" s="325">
-        <f>N232*1.05</f>
-        <v>1.4398895185724963</v>
+        <f>N232</f>
+        <v>1.3713233510214249</v>
       </c>
     </row>
     <row r="253" spans="1:25" x14ac:dyDescent="0.25">
@@ -33659,7 +33659,8 @@
         <v>498</v>
       </c>
       <c r="D257" s="303">
-        <v>129.54169999999999</v>
+        <f>129.5417*1.56</f>
+        <v>202.08505199999999</v>
       </c>
       <c r="E257" s="302">
         <f>5/0.14</f>
@@ -33690,7 +33691,8 @@
         <v>494</v>
       </c>
       <c r="D258" s="303">
-        <v>12.8826</v>
+        <f>12.8826*1.56</f>
+        <v>20.096856000000002</v>
       </c>
       <c r="E258" s="302">
         <f>0.04*E257</f>
@@ -33722,7 +33724,7 @@
       </c>
       <c r="D259" s="176">
         <f>E259/E257 *D257</f>
-        <v>14.249587000000002</v>
+        <v>22.229355720000001</v>
       </c>
       <c r="E259" s="302">
         <f>0.55/0.14</f>
@@ -33822,7 +33824,7 @@
       </c>
       <c r="N263" s="299">
         <f>D259</f>
-        <v>14.249587000000002</v>
+        <v>22.229355720000001</v>
       </c>
     </row>
     <row r="264" spans="2:14" x14ac:dyDescent="0.25">
@@ -33847,7 +33849,7 @@
       </c>
       <c r="N264" s="299">
         <f>D257</f>
-        <v>129.54169999999999</v>
+        <v>202.08505199999999</v>
       </c>
     </row>
     <row r="265" spans="2:14" x14ac:dyDescent="0.25">
@@ -33872,7 +33874,7 @@
       </c>
       <c r="N265" s="299">
         <f>D258</f>
-        <v>12.8826</v>
+        <v>20.096856000000002</v>
       </c>
     </row>
     <row r="266" spans="2:14" x14ac:dyDescent="0.25">
@@ -33893,7 +33895,7 @@
         <v>492</v>
       </c>
       <c r="N266" s="298">
-        <v>2025</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="267" spans="2:14" x14ac:dyDescent="0.25">
@@ -34201,7 +34203,7 @@
       </c>
       <c r="K282" s="278">
         <f ca="1">SUMIF($J$37:$J$269,K$278&amp;$A282,$N$37:$N$245)</f>
-        <v>1.4398895185724963</v>
+        <v>1.3713233510214249</v>
       </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.25">
@@ -34244,7 +34246,7 @@
       </c>
       <c r="K283" s="276">
         <f ca="1">SUMIF($J$37:$J$269,K$278&amp;$A283,$N$37:$N$245)</f>
-        <v>27.132187000000002</v>
+        <v>42.326211720000003</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
@@ -34287,7 +34289,7 @@
       </c>
       <c r="K284" s="276">
         <f ca="1">SUMIF($J$37:$J$269,K$278&amp;$A284,$N$37:$N$245)</f>
-        <v>129.54169999999999</v>
+        <v>202.08505199999999</v>
       </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.25">
@@ -34451,26 +34453,26 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="96" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="486" t="s">
+      <c r="C2" s="496" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="487"/>
-      <c r="E2" s="487"/>
-      <c r="F2" s="488" t="s">
+      <c r="D2" s="497"/>
+      <c r="E2" s="497"/>
+      <c r="F2" s="498" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="489"/>
-      <c r="H2" s="490"/>
-      <c r="I2" s="488" t="s">
+      <c r="G2" s="499"/>
+      <c r="H2" s="500"/>
+      <c r="I2" s="498" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="489"/>
-      <c r="K2" s="490"/>
-      <c r="L2" s="488" t="s">
+      <c r="J2" s="499"/>
+      <c r="K2" s="500"/>
+      <c r="L2" s="498" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="489"/>
-      <c r="N2" s="490"/>
+      <c r="M2" s="499"/>
+      <c r="N2" s="500"/>
       <c r="O2" s="97"/>
       <c r="P2" s="13"/>
       <c r="AA2" s="96" t="s">
@@ -34743,10 +34745,10 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="491" t="s">
+      <c r="A9" s="485" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="492"/>
+      <c r="B9" s="486"/>
       <c r="C9" s="49"/>
       <c r="D9" s="44">
         <f>D5/$O$5</f>
@@ -34771,49 +34773,49 @@
       <c r="O9" s="7">
         <v>788</v>
       </c>
-      <c r="Q9" s="497" t="s">
+      <c r="Q9" s="491" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="499" t="s">
+      <c r="S9" s="493" t="s">
         <v>83</v>
       </c>
-      <c r="V9" s="495" t="s">
+      <c r="V9" s="489" t="s">
         <v>881</v>
       </c>
-      <c r="W9" s="495" t="s">
+      <c r="W9" s="489" t="s">
         <v>882</v>
       </c>
-      <c r="X9" s="495" t="s">
+      <c r="X9" s="489" t="s">
         <v>82</v>
       </c>
-      <c r="Y9" s="495" t="s">
+      <c r="Y9" s="489" t="s">
         <v>883</v>
       </c>
-      <c r="Z9" s="495" t="s">
+      <c r="Z9" s="489" t="s">
         <v>884</v>
       </c>
-      <c r="AA9" s="495" t="s">
+      <c r="AA9" s="489" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="495" t="s">
+      <c r="AB9" s="489" t="s">
         <v>885</v>
       </c>
-      <c r="AC9" s="495" t="s">
+      <c r="AC9" s="489" t="s">
         <v>886</v>
       </c>
-      <c r="AD9" s="495" t="s">
+      <c r="AD9" s="489" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="495" t="s">
+      <c r="AE9" s="489" t="s">
         <v>887</v>
       </c>
-      <c r="AF9" s="495" t="s">
+      <c r="AF9" s="489" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="493"/>
-      <c r="B10" s="494"/>
+      <c r="A10" s="487"/>
+      <c r="B10" s="488"/>
       <c r="C10" s="49"/>
       <c r="D10" s="9">
         <f>D9*788</f>
@@ -34839,25 +34841,25 @@
         <f>O9-G10</f>
         <v>422.2729198252656</v>
       </c>
-      <c r="Q10" s="498"/>
+      <c r="Q10" s="492"/>
       <c r="R10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="S10" s="500"/>
+      <c r="S10" s="494"/>
       <c r="U10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="V10" s="496"/>
-      <c r="W10" s="496"/>
-      <c r="X10" s="496"/>
-      <c r="Y10" s="496"/>
-      <c r="Z10" s="496"/>
-      <c r="AA10" s="496"/>
-      <c r="AB10" s="496"/>
-      <c r="AC10" s="496"/>
-      <c r="AD10" s="496"/>
-      <c r="AE10" s="496"/>
-      <c r="AF10" s="496"/>
+      <c r="V10" s="490"/>
+      <c r="W10" s="490"/>
+      <c r="X10" s="490"/>
+      <c r="Y10" s="490"/>
+      <c r="Z10" s="490"/>
+      <c r="AA10" s="490"/>
+      <c r="AB10" s="490"/>
+      <c r="AC10" s="490"/>
+      <c r="AD10" s="490"/>
+      <c r="AE10" s="490"/>
+      <c r="AF10" s="490"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
@@ -37349,11 +37351,11 @@
       <c r="J62" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="485" t="s">
+      <c r="K62" s="495" t="s">
         <v>26</v>
       </c>
-      <c r="L62" s="485"/>
-      <c r="M62" s="485"/>
+      <c r="L62" s="495"/>
+      <c r="M62" s="495"/>
       <c r="N62"/>
     </row>
     <row r="63" spans="3:22" ht="15" x14ac:dyDescent="0.25">
@@ -37611,6 +37613,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AC9:AC10"/>
@@ -37625,11 +37632,6 @@
     <mergeCell ref="AB9:AB10"/>
     <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="W9:W10"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40298,7 +40300,7 @@
         <v>190</v>
       </c>
       <c r="G2" s="509"/>
-      <c r="H2" s="490"/>
+      <c r="H2" s="500"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -40540,7 +40542,7 @@
       <c r="G14" s="88"/>
       <c r="H14" s="154"/>
       <c r="I14" s="153"/>
-      <c r="J14" s="500"/>
+      <c r="J14" s="494"/>
       <c r="K14" s="152" t="s">
         <v>79</v>
       </c>
@@ -44428,27 +44430,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="513" t="s">
+      <c r="A1" s="521" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
+      <c r="B1" s="516"/>
+      <c r="C1" s="516"/>
+      <c r="D1" s="516"/>
+      <c r="E1" s="516"/>
+      <c r="F1" s="516"/>
+      <c r="G1" s="516"/>
+      <c r="H1" s="516"/>
+      <c r="I1" s="516"/>
       <c r="J1" s="216" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="515" t="s">
+      <c r="A2" s="522" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="515"/>
-      <c r="C2" s="515"/>
+      <c r="B2" s="522"/>
+      <c r="C2" s="522"/>
       <c r="D2" s="259">
         <v>2019</v>
       </c>
@@ -44485,16 +44487,16 @@
       <c r="U2" s="252"/>
     </row>
     <row r="3" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="516" t="s">
+      <c r="A3" s="523" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="516"/>
+      <c r="B3" s="523"/>
       <c r="C3" s="254"/>
       <c r="D3" s="255"/>
       <c r="E3" s="254"/>
       <c r="F3" s="254"/>
       <c r="G3" s="253"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="524" t="s">
         <v>373</v>
       </c>
       <c r="Q3"/>
@@ -44504,10 +44506,10 @@
       <c r="U3" s="252"/>
     </row>
     <row r="4" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="520" t="s">
+      <c r="A4" s="527" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="520"/>
+      <c r="B4" s="527"/>
       <c r="C4" s="241">
         <v>1</v>
       </c>
@@ -44523,7 +44525,7 @@
       <c r="G4" s="221">
         <v>18806</v>
       </c>
-      <c r="H4" s="518"/>
+      <c r="H4" s="525"/>
       <c r="J4" s="216">
         <f>D4/F4</f>
         <v>0.99859246427024684</v>
@@ -44541,10 +44543,10 @@
       <c r="T4" s="252"/>
     </row>
     <row r="5" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="521" t="s">
+      <c r="A5" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="521"/>
+      <c r="B5" s="513"/>
       <c r="C5" s="239"/>
       <c r="D5" s="231">
         <v>6736</v>
@@ -44558,13 +44560,13 @@
       <c r="G5" s="221">
         <v>7019</v>
       </c>
-      <c r="H5" s="518"/>
+      <c r="H5" s="525"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="521" t="s">
+      <c r="A6" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="521"/>
+      <c r="B6" s="513"/>
       <c r="C6" s="239"/>
       <c r="D6" s="231">
         <v>1467</v>
@@ -44578,13 +44580,13 @@
       <c r="G6" s="221">
         <v>1461</v>
       </c>
-      <c r="H6" s="518"/>
+      <c r="H6" s="525"/>
     </row>
     <row r="7" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="521" t="s">
+      <c r="A7" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="521"/>
+      <c r="B7" s="513"/>
       <c r="C7" s="239"/>
       <c r="D7" s="231">
         <v>3209</v>
@@ -44598,13 +44600,13 @@
       <c r="G7" s="221">
         <v>3331</v>
       </c>
-      <c r="H7" s="518"/>
+      <c r="H7" s="525"/>
     </row>
     <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="521" t="s">
+      <c r="A8" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B8" s="521"/>
+      <c r="B8" s="513"/>
       <c r="C8" s="239"/>
       <c r="D8" s="231">
         <v>4271</v>
@@ -44618,13 +44620,13 @@
       <c r="G8" s="221">
         <v>4067</v>
       </c>
-      <c r="H8" s="518"/>
+      <c r="H8" s="525"/>
     </row>
     <row r="9" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="521" t="s">
+      <c r="A9" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="521"/>
+      <c r="B9" s="513"/>
       <c r="C9" s="239"/>
       <c r="D9" s="231">
         <v>1277</v>
@@ -44638,13 +44640,13 @@
       <c r="G9" s="221">
         <v>1309</v>
       </c>
-      <c r="H9" s="518"/>
+      <c r="H9" s="525"/>
     </row>
     <row r="10" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="521" t="s">
+      <c r="A10" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="521"/>
+      <c r="B10" s="513"/>
       <c r="C10" s="239"/>
       <c r="D10" s="233">
         <v>688</v>
@@ -44658,13 +44660,13 @@
       <c r="G10" s="218">
         <v>793</v>
       </c>
-      <c r="H10" s="518"/>
+      <c r="H10" s="525"/>
     </row>
     <row r="11" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="521" t="s">
+      <c r="A11" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="521"/>
+      <c r="B11" s="513"/>
       <c r="C11" s="239"/>
       <c r="D11" s="233">
         <v>53</v>
@@ -44678,14 +44680,14 @@
       <c r="G11" s="218">
         <v>62</v>
       </c>
-      <c r="H11" s="518"/>
+      <c r="H11" s="525"/>
     </row>
     <row r="12" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="522" t="s">
+      <c r="A12" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B12" s="522"/>
-      <c r="C12" s="522"/>
+      <c r="B12" s="514"/>
+      <c r="C12" s="514"/>
       <c r="D12" s="251">
         <v>745</v>
       </c>
@@ -44698,14 +44700,14 @@
       <c r="G12" s="249">
         <v>763</v>
       </c>
-      <c r="H12" s="519"/>
+      <c r="H12" s="526"/>
       <c r="V12" s="243"/>
     </row>
     <row r="13" spans="1:22" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="523" t="s">
+      <c r="A13" s="520" t="s">
         <v>396</v>
       </c>
-      <c r="B13" s="523"/>
+      <c r="B13" s="520"/>
       <c r="C13" s="248">
         <v>2</v>
       </c>
@@ -44717,10 +44719,10 @@
       <c r="V13" s="243"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="514" t="s">
+      <c r="A14" s="516" t="s">
         <v>395</v>
       </c>
-      <c r="B14" s="514"/>
+      <c r="B14" s="516"/>
       <c r="C14" s="239"/>
       <c r="D14" s="231">
         <v>105.04</v>
@@ -44755,10 +44757,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="521" t="s">
+      <c r="A15" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="521"/>
+      <c r="B15" s="513"/>
       <c r="C15" s="239"/>
       <c r="D15" s="231">
         <v>96.16</v>
@@ -44791,10 +44793,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="521" t="s">
+      <c r="A16" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="521"/>
+      <c r="B16" s="513"/>
       <c r="C16" s="239"/>
       <c r="D16" s="231">
         <v>5.34</v>
@@ -44827,10 +44829,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="521" t="s">
+      <c r="A17" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B17" s="521"/>
+      <c r="B17" s="513"/>
       <c r="C17" s="239"/>
       <c r="D17" s="231">
         <v>3.49</v>
@@ -44863,10 +44865,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="521" t="s">
+      <c r="A18" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B18" s="521"/>
+      <c r="B18" s="513"/>
       <c r="C18" s="239"/>
       <c r="D18" s="242">
         <v>0</v>
@@ -44899,10 +44901,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="521" t="s">
+      <c r="A19" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="521"/>
+      <c r="B19" s="513"/>
       <c r="C19" s="239"/>
       <c r="D19" s="231">
         <v>0</v>
@@ -44935,10 +44937,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="521" t="s">
+      <c r="A20" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B20" s="521"/>
+      <c r="B20" s="513"/>
       <c r="C20" s="239"/>
       <c r="D20" s="231">
         <v>0.04</v>
@@ -44971,10 +44973,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="521" t="s">
+      <c r="A21" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B21" s="521"/>
+      <c r="B21" s="513"/>
       <c r="C21" s="239"/>
       <c r="D21" s="231">
         <v>0</v>
@@ -45007,11 +45009,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="521" t="s">
+      <c r="A22" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B22" s="521"/>
-      <c r="C22" s="521"/>
+      <c r="B22" s="513"/>
+      <c r="C22" s="513"/>
       <c r="D22" s="231">
         <v>0.01</v>
       </c>
@@ -45043,10 +45045,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="514" t="s">
+      <c r="A23" s="516" t="s">
         <v>394</v>
       </c>
-      <c r="B23" s="514"/>
+      <c r="B23" s="516"/>
       <c r="C23" s="239"/>
       <c r="D23" s="231">
         <v>1.64</v>
@@ -45081,10 +45083,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="521" t="s">
+      <c r="A24" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B24" s="521"/>
+      <c r="B24" s="513"/>
       <c r="C24" s="239"/>
       <c r="D24" s="231">
         <v>0.9</v>
@@ -45117,10 +45119,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="521" t="s">
+      <c r="A25" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="521"/>
+      <c r="B25" s="513"/>
       <c r="C25" s="239"/>
       <c r="D25" s="231">
         <v>0.73</v>
@@ -45153,10 +45155,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="521" t="s">
+      <c r="A26" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B26" s="521"/>
+      <c r="B26" s="513"/>
       <c r="C26" s="239"/>
       <c r="D26" s="231">
         <v>0</v>
@@ -45189,10 +45191,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="521" t="s">
+      <c r="A27" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B27" s="521"/>
+      <c r="B27" s="513"/>
       <c r="C27" s="239"/>
       <c r="D27" s="231">
         <v>0</v>
@@ -45225,10 +45227,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="521" t="s">
+      <c r="A28" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="521"/>
+      <c r="B28" s="513"/>
       <c r="C28" s="239"/>
       <c r="D28" s="231">
         <v>0</v>
@@ -45261,10 +45263,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="521" t="s">
+      <c r="A29" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B29" s="521"/>
+      <c r="B29" s="513"/>
       <c r="C29" s="239"/>
       <c r="D29" s="231">
         <v>0.01</v>
@@ -45297,10 +45299,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="521" t="s">
+      <c r="A30" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B30" s="521"/>
+      <c r="B30" s="513"/>
       <c r="C30" s="239"/>
       <c r="D30" s="231">
         <v>0</v>
@@ -45333,11 +45335,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="521" t="s">
+      <c r="A31" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B31" s="521"/>
-      <c r="C31" s="521"/>
+      <c r="B31" s="513"/>
+      <c r="C31" s="513"/>
       <c r="D31" s="231">
         <v>0</v>
       </c>
@@ -45369,10 +45371,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="514" t="s">
+      <c r="A32" s="516" t="s">
         <v>393</v>
       </c>
-      <c r="B32" s="514"/>
+      <c r="B32" s="516"/>
       <c r="C32" s="239"/>
       <c r="D32" s="231">
         <v>56004</v>
@@ -45407,10 +45409,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="521" t="s">
+      <c r="A33" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B33" s="521"/>
+      <c r="B33" s="513"/>
       <c r="C33" s="239"/>
       <c r="D33" s="231">
         <v>48418</v>
@@ -45449,10 +45451,10 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="521" t="s">
+      <c r="A34" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="521"/>
+      <c r="B34" s="513"/>
       <c r="C34" s="239"/>
       <c r="D34" s="231">
         <v>4557</v>
@@ -45485,10 +45487,10 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="521" t="s">
+      <c r="A35" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B35" s="521"/>
+      <c r="B35" s="513"/>
       <c r="C35" s="239"/>
       <c r="D35" s="233">
         <v>16</v>
@@ -45521,10 +45523,10 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="521" t="s">
+      <c r="A36" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B36" s="521"/>
+      <c r="B36" s="513"/>
       <c r="C36" s="239"/>
       <c r="D36" s="233">
         <v>932</v>
@@ -45557,10 +45559,10 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="521" t="s">
+      <c r="A37" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B37" s="521"/>
+      <c r="B37" s="513"/>
       <c r="C37" s="239"/>
       <c r="D37" s="233">
         <v>610</v>
@@ -45593,10 +45595,10 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="521" t="s">
+      <c r="A38" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="521"/>
+      <c r="B38" s="513"/>
       <c r="C38" s="239"/>
       <c r="D38" s="231">
         <v>1163</v>
@@ -45629,10 +45631,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="521" t="s">
+      <c r="A39" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B39" s="521"/>
+      <c r="B39" s="513"/>
       <c r="C39" s="239"/>
       <c r="D39" s="233">
         <v>261</v>
@@ -45665,11 +45667,11 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="521" t="s">
+      <c r="A40" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B40" s="521"/>
-      <c r="C40" s="521"/>
+      <c r="B40" s="513"/>
+      <c r="C40" s="513"/>
       <c r="D40" s="233">
         <v>47</v>
       </c>
@@ -45701,10 +45703,10 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="514" t="s">
+      <c r="A41" s="516" t="s">
         <v>391</v>
       </c>
-      <c r="B41" s="514"/>
+      <c r="B41" s="516"/>
       <c r="C41" s="241">
         <v>3</v>
       </c>
@@ -45725,10 +45727,10 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="521" t="s">
+      <c r="A42" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B42" s="521"/>
+      <c r="B42" s="513"/>
       <c r="C42" s="239"/>
       <c r="D42" s="231">
         <v>5596</v>
@@ -45764,10 +45766,10 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="521" t="s">
+      <c r="A43" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="521"/>
+      <c r="B43" s="513"/>
       <c r="C43" s="239"/>
       <c r="D43" s="233">
         <v>400</v>
@@ -45803,10 +45805,10 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="521" t="s">
+      <c r="A44" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B44" s="521"/>
+      <c r="B44" s="513"/>
       <c r="C44" s="239"/>
       <c r="D44" s="233">
         <v>726</v>
@@ -45842,10 +45844,10 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="521" t="s">
+      <c r="A45" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="521"/>
+      <c r="B45" s="513"/>
       <c r="C45" s="239"/>
       <c r="D45" s="233">
         <v>289</v>
@@ -45881,10 +45883,10 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="521" t="s">
+      <c r="A46" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B46" s="521"/>
+      <c r="B46" s="513"/>
       <c r="C46" s="239"/>
       <c r="D46" s="233">
         <v>108</v>
@@ -45901,10 +45903,10 @@
       <c r="H46" s="230"/>
     </row>
     <row r="47" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="521" t="s">
+      <c r="A47" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="521"/>
+      <c r="B47" s="513"/>
       <c r="C47" s="239"/>
       <c r="D47" s="233">
         <v>498</v>
@@ -45921,10 +45923,10 @@
       <c r="H47" s="230"/>
     </row>
     <row r="48" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="521" t="s">
+      <c r="A48" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="521"/>
+      <c r="B48" s="513"/>
       <c r="C48" s="239"/>
       <c r="D48" s="231">
         <v>0</v>
@@ -45941,11 +45943,11 @@
       <c r="H48" s="230"/>
     </row>
     <row r="49" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="521" t="s">
+      <c r="A49" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="521"/>
-      <c r="C49" s="521"/>
+      <c r="B49" s="513"/>
+      <c r="C49" s="513"/>
       <c r="D49" s="233">
         <v>36</v>
       </c>
@@ -45961,10 +45963,10 @@
       <c r="H49" s="230"/>
     </row>
     <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="514" t="s">
+      <c r="A50" s="516" t="s">
         <v>390</v>
       </c>
-      <c r="B50" s="514"/>
+      <c r="B50" s="516"/>
       <c r="C50" s="241">
         <v>4</v>
       </c>
@@ -45985,10 +45987,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="521" t="s">
+      <c r="A51" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B51" s="521"/>
+      <c r="B51" s="513"/>
       <c r="C51" s="239"/>
       <c r="D51" s="231">
         <v>0</v>
@@ -46005,10 +46007,10 @@
       <c r="H51" s="230"/>
     </row>
     <row r="52" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="521" t="s">
+      <c r="A52" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B52" s="521"/>
+      <c r="B52" s="513"/>
       <c r="C52" s="239"/>
       <c r="D52" s="231">
         <v>0</v>
@@ -46025,10 +46027,10 @@
       <c r="H52" s="230"/>
     </row>
     <row r="53" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="521" t="s">
+      <c r="A53" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B53" s="521"/>
+      <c r="B53" s="513"/>
       <c r="C53" s="239"/>
       <c r="D53" s="231">
         <v>0</v>
@@ -46045,10 +46047,10 @@
       <c r="H53" s="230"/>
     </row>
     <row r="54" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="521" t="s">
+      <c r="A54" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B54" s="521"/>
+      <c r="B54" s="513"/>
       <c r="C54" s="239"/>
       <c r="D54" s="231">
         <v>0</v>
@@ -46065,10 +46067,10 @@
       <c r="H54" s="230"/>
     </row>
     <row r="55" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="521" t="s">
+      <c r="A55" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B55" s="521"/>
+      <c r="B55" s="513"/>
       <c r="C55" s="239"/>
       <c r="D55" s="231">
         <v>0</v>
@@ -46085,10 +46087,10 @@
       <c r="H55" s="230"/>
     </row>
     <row r="56" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="521" t="s">
+      <c r="A56" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B56" s="521"/>
+      <c r="B56" s="513"/>
       <c r="C56" s="239"/>
       <c r="D56" s="231">
         <v>0</v>
@@ -46105,10 +46107,10 @@
       <c r="H56" s="230"/>
     </row>
     <row r="57" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="521" t="s">
+      <c r="A57" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="521"/>
+      <c r="B57" s="513"/>
       <c r="C57" s="239"/>
       <c r="D57" s="231">
         <v>0.05</v>
@@ -46125,11 +46127,11 @@
       <c r="H57" s="230"/>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="522" t="s">
+      <c r="A58" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B58" s="522"/>
-      <c r="C58" s="522"/>
+      <c r="B58" s="514"/>
+      <c r="C58" s="514"/>
       <c r="D58" s="229">
         <v>0</v>
       </c>
@@ -46145,46 +46147,46 @@
       <c r="H58" s="238"/>
     </row>
     <row r="59" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="514"/>
-      <c r="B59" s="514"/>
-      <c r="C59" s="514"/>
-      <c r="D59" s="514"/>
-      <c r="E59" s="514"/>
-      <c r="F59" s="514"/>
-      <c r="G59" s="514"/>
-      <c r="H59" s="514"/>
-      <c r="I59" s="514"/>
+      <c r="A59" s="516"/>
+      <c r="B59" s="516"/>
+      <c r="C59" s="516"/>
+      <c r="D59" s="516"/>
+      <c r="E59" s="516"/>
+      <c r="F59" s="516"/>
+      <c r="G59" s="516"/>
+      <c r="H59" s="516"/>
+      <c r="I59" s="516"/>
     </row>
     <row r="60" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="514"/>
-      <c r="B60" s="514"/>
-      <c r="C60" s="514"/>
-      <c r="D60" s="514"/>
-      <c r="E60" s="514"/>
-      <c r="F60" s="514"/>
-      <c r="G60" s="514"/>
-      <c r="H60" s="514"/>
-      <c r="I60" s="514"/>
+      <c r="A60" s="516"/>
+      <c r="B60" s="516"/>
+      <c r="C60" s="516"/>
+      <c r="D60" s="516"/>
+      <c r="E60" s="516"/>
+      <c r="F60" s="516"/>
+      <c r="G60" s="516"/>
+      <c r="H60" s="516"/>
+      <c r="I60" s="516"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="524" t="s">
+      <c r="A61" s="519" t="s">
         <v>388</v>
       </c>
-      <c r="B61" s="524"/>
-      <c r="C61" s="524"/>
-      <c r="D61" s="524"/>
-      <c r="E61" s="524"/>
-      <c r="F61" s="524"/>
-      <c r="G61" s="524"/>
-      <c r="H61" s="524"/>
-      <c r="I61" s="524"/>
+      <c r="B61" s="519"/>
+      <c r="C61" s="519"/>
+      <c r="D61" s="519"/>
+      <c r="E61" s="519"/>
+      <c r="F61" s="519"/>
+      <c r="G61" s="519"/>
+      <c r="H61" s="519"/>
+      <c r="I61" s="519"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="525" t="s">
+      <c r="A62" s="517" t="s">
         <v>345</v>
       </c>
-      <c r="B62" s="525"/>
-      <c r="C62" s="525"/>
+      <c r="B62" s="517"/>
+      <c r="C62" s="517"/>
       <c r="D62" s="225">
         <v>2019</v>
       </c>
@@ -46202,11 +46204,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="526" t="s">
+      <c r="A63" s="518" t="s">
         <v>344</v>
       </c>
-      <c r="B63" s="526"/>
-      <c r="C63" s="526"/>
+      <c r="B63" s="518"/>
+      <c r="C63" s="518"/>
       <c r="D63" s="220" t="s">
         <v>386</v>
       </c>
@@ -46224,11 +46226,11 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="521" t="s">
+      <c r="A64" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="521"/>
-      <c r="C64" s="521"/>
+      <c r="B64" s="513"/>
+      <c r="C64" s="513"/>
       <c r="D64" s="231" t="s">
         <v>382</v>
       </c>
@@ -46244,11 +46246,11 @@
       <c r="H64" s="230"/>
     </row>
     <row r="65" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="521" t="s">
+      <c r="A65" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B65" s="521"/>
-      <c r="C65" s="521"/>
+      <c r="B65" s="513"/>
+      <c r="C65" s="513"/>
       <c r="D65" s="231" t="s">
         <v>380</v>
       </c>
@@ -46264,11 +46266,11 @@
       <c r="H65" s="230"/>
     </row>
     <row r="66" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="521" t="s">
+      <c r="A66" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B66" s="521"/>
-      <c r="C66" s="521"/>
+      <c r="B66" s="513"/>
+      <c r="C66" s="513"/>
       <c r="D66" s="233">
         <v>822</v>
       </c>
@@ -46284,11 +46286,11 @@
       <c r="H66" s="230"/>
     </row>
     <row r="67" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="521" t="s">
+      <c r="A67" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B67" s="521"/>
-      <c r="C67" s="521"/>
+      <c r="B67" s="513"/>
+      <c r="C67" s="513"/>
       <c r="D67" s="231" t="s">
         <v>379</v>
       </c>
@@ -46304,11 +46306,11 @@
       <c r="H67" s="230"/>
     </row>
     <row r="68" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="521" t="s">
+      <c r="A68" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="521"/>
-      <c r="C68" s="521"/>
+      <c r="B68" s="513"/>
+      <c r="C68" s="513"/>
       <c r="D68" s="233">
         <v>717</v>
       </c>
@@ -46324,11 +46326,11 @@
       <c r="H68" s="230"/>
     </row>
     <row r="69" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="521" t="s">
+      <c r="A69" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="521"/>
-      <c r="C69" s="521"/>
+      <c r="B69" s="513"/>
+      <c r="C69" s="513"/>
       <c r="D69" s="231" t="s">
         <v>378</v>
       </c>
@@ -46344,11 +46346,11 @@
       <c r="H69" s="230"/>
     </row>
     <row r="70" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="521" t="s">
+      <c r="A70" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B70" s="521"/>
-      <c r="C70" s="521"/>
+      <c r="B70" s="513"/>
+      <c r="C70" s="513"/>
       <c r="D70" s="233">
         <v>261</v>
       </c>
@@ -46364,11 +46366,11 @@
       <c r="H70" s="230"/>
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="521" t="s">
+      <c r="A71" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B71" s="521"/>
-      <c r="C71" s="521"/>
+      <c r="B71" s="513"/>
+      <c r="C71" s="513"/>
       <c r="D71" s="233">
         <v>83</v>
       </c>
@@ -46384,11 +46386,11 @@
       <c r="H71" s="230"/>
     </row>
     <row r="72" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="514" t="s">
+      <c r="A72" s="516" t="s">
         <v>377</v>
       </c>
-      <c r="B72" s="514"/>
-      <c r="C72" s="514"/>
+      <c r="B72" s="516"/>
+      <c r="C72" s="516"/>
       <c r="D72" s="231" t="s">
         <v>368</v>
       </c>
@@ -46406,11 +46408,11 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="521" t="s">
+      <c r="A73" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B73" s="521"/>
-      <c r="C73" s="521"/>
+      <c r="B73" s="513"/>
+      <c r="C73" s="513"/>
       <c r="D73" s="231" t="s">
         <v>372</v>
       </c>
@@ -46426,11 +46428,11 @@
       <c r="H73" s="230"/>
     </row>
     <row r="74" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="521" t="s">
+      <c r="A74" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B74" s="521"/>
-      <c r="C74" s="521"/>
+      <c r="B74" s="513"/>
+      <c r="C74" s="513"/>
       <c r="D74" s="231" t="s">
         <v>368</v>
       </c>
@@ -46446,11 +46448,11 @@
       <c r="H74" s="230"/>
     </row>
     <row r="75" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="521" t="s">
+      <c r="A75" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B75" s="521"/>
-      <c r="C75" s="521"/>
+      <c r="B75" s="513"/>
+      <c r="C75" s="513"/>
       <c r="D75" s="231" t="s">
         <v>348</v>
       </c>
@@ -46466,11 +46468,11 @@
       <c r="H75" s="230"/>
     </row>
     <row r="76" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="521" t="s">
+      <c r="A76" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B76" s="521"/>
-      <c r="C76" s="521"/>
+      <c r="B76" s="513"/>
+      <c r="C76" s="513"/>
       <c r="D76" s="231" t="s">
         <v>362</v>
       </c>
@@ -46486,11 +46488,11 @@
       <c r="H76" s="230"/>
     </row>
     <row r="77" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="521" t="s">
+      <c r="A77" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B77" s="521"/>
-      <c r="C77" s="521"/>
+      <c r="B77" s="513"/>
+      <c r="C77" s="513"/>
       <c r="D77" s="231" t="s">
         <v>361</v>
       </c>
@@ -46506,11 +46508,11 @@
       <c r="H77" s="230"/>
     </row>
     <row r="78" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="521" t="s">
+      <c r="A78" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B78" s="521"/>
-      <c r="C78" s="521"/>
+      <c r="B78" s="513"/>
+      <c r="C78" s="513"/>
       <c r="D78" s="231" t="s">
         <v>358</v>
       </c>
@@ -46526,11 +46528,11 @@
       <c r="H78" s="230"/>
     </row>
     <row r="79" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="521" t="s">
+      <c r="A79" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="521"/>
-      <c r="C79" s="521"/>
+      <c r="B79" s="513"/>
+      <c r="C79" s="513"/>
       <c r="D79" s="231" t="s">
         <v>354</v>
       </c>
@@ -46546,11 +46548,11 @@
       <c r="H79" s="230"/>
     </row>
     <row r="80" spans="1:8" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="522" t="s">
+      <c r="A80" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B80" s="522"/>
-      <c r="C80" s="522"/>
+      <c r="B80" s="514"/>
+      <c r="C80" s="514"/>
       <c r="D80" s="229" t="s">
         <v>349</v>
       </c>
@@ -46566,30 +46568,30 @@
       <c r="H80" s="226"/>
     </row>
     <row r="81" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="527" t="s">
+      <c r="A81" s="515" t="s">
         <v>347</v>
       </c>
-      <c r="B81" s="514"/>
-      <c r="C81" s="514"/>
-      <c r="D81" s="514"/>
-      <c r="E81" s="514"/>
-      <c r="F81" s="514"/>
-      <c r="G81" s="514"/>
-      <c r="H81" s="514"/>
-      <c r="I81" s="514"/>
+      <c r="B81" s="516"/>
+      <c r="C81" s="516"/>
+      <c r="D81" s="516"/>
+      <c r="E81" s="516"/>
+      <c r="F81" s="516"/>
+      <c r="G81" s="516"/>
+      <c r="H81" s="516"/>
+      <c r="I81" s="516"/>
     </row>
     <row r="82" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="514" t="s">
+      <c r="A82" s="516" t="s">
         <v>346</v>
       </c>
-      <c r="B82" s="514"/>
-      <c r="C82" s="514"/>
-      <c r="D82" s="514"/>
-      <c r="E82" s="514"/>
-      <c r="F82" s="514"/>
-      <c r="G82" s="514"/>
-      <c r="H82" s="514"/>
-      <c r="I82" s="514"/>
+      <c r="B82" s="516"/>
+      <c r="C82" s="516"/>
+      <c r="D82" s="516"/>
+      <c r="E82" s="516"/>
+      <c r="F82" s="516"/>
+      <c r="G82" s="516"/>
+      <c r="H82" s="516"/>
+      <c r="I82" s="516"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D83" s="216" t="str">
@@ -46610,11 +46612,11 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="525" t="s">
+      <c r="A85" s="517" t="s">
         <v>345</v>
       </c>
-      <c r="B85" s="525"/>
-      <c r="C85" s="525"/>
+      <c r="B85" s="517"/>
+      <c r="C85" s="517"/>
       <c r="D85" s="225">
         <v>2019</v>
       </c>
@@ -46641,11 +46643,11 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="526" t="s">
+      <c r="A86" s="518" t="s">
         <v>344</v>
       </c>
-      <c r="B86" s="526"/>
-      <c r="C86" s="526"/>
+      <c r="B86" s="518"/>
+      <c r="C86" s="518"/>
       <c r="D86" s="220">
         <f>D14*gwpch4+D23*gwpn2o+D32+D41+D50</f>
         <v>66558.41</v>
@@ -46683,11 +46685,11 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="521" t="s">
+      <c r="A87" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B87" s="521"/>
-      <c r="C87" s="521"/>
+      <c r="B87" s="513"/>
+      <c r="C87" s="513"/>
       <c r="D87" s="220">
         <f t="shared" ref="D87:D94" si="14">D15*gwpch4+D24*gwpn2o+D33+D42+D51</f>
         <v>56492.08</v>
@@ -46722,11 +46724,11 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="521" t="s">
+      <c r="A88" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B88" s="521"/>
-      <c r="C88" s="521"/>
+      <c r="B88" s="513"/>
+      <c r="C88" s="513"/>
       <c r="D88" s="220">
         <f t="shared" si="14"/>
         <v>5295.9</v>
@@ -46761,11 +46763,11 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="521" t="s">
+      <c r="A89" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B89" s="521"/>
-      <c r="C89" s="521"/>
+      <c r="B89" s="513"/>
+      <c r="C89" s="513"/>
       <c r="D89" s="220">
         <f t="shared" si="14"/>
         <v>822.27</v>
@@ -46800,11 +46802,11 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="521" t="s">
+      <c r="A90" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B90" s="521"/>
-      <c r="C90" s="521"/>
+      <c r="B90" s="513"/>
+      <c r="C90" s="513"/>
       <c r="D90" s="220">
         <f t="shared" si="14"/>
         <v>1221</v>
@@ -46839,11 +46841,11 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="521" t="s">
+      <c r="A91" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B91" s="521"/>
-      <c r="C91" s="521"/>
+      <c r="B91" s="513"/>
+      <c r="C91" s="513"/>
       <c r="D91" s="220">
         <f t="shared" si="14"/>
         <v>718</v>
@@ -46878,11 +46880,11 @@
       </c>
     </row>
     <row r="92" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="521" t="s">
+      <c r="A92" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B92" s="521"/>
-      <c r="C92" s="521"/>
+      <c r="B92" s="513"/>
+      <c r="C92" s="513"/>
       <c r="D92" s="220">
         <f t="shared" si="14"/>
         <v>1664.88</v>
@@ -46917,11 +46919,11 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="521" t="s">
+      <c r="A93" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B93" s="521"/>
-      <c r="C93" s="521"/>
+      <c r="B93" s="513"/>
+      <c r="C93" s="513"/>
       <c r="D93" s="220">
         <f t="shared" si="14"/>
         <v>261.05</v>
@@ -46956,11 +46958,11 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="521" t="s">
+      <c r="A94" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B94" s="521"/>
-      <c r="C94" s="521"/>
+      <c r="B94" s="513"/>
+      <c r="C94" s="513"/>
       <c r="D94" s="220">
         <f t="shared" si="14"/>
         <v>83.22999999999999</v>
@@ -47044,38 +47046,51 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A94:C94"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="A59:I59"/>
@@ -47092,51 +47107,38 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:H12"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A94:C94"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A81" r:id="rId1" display="http://www.sasol.com/" xr:uid="{94E57AF8-CF1E-4A4A-992A-3647A9F5048E}"/>

</xml_diff>

<commit_message>
More fixes to gas supply
</commit_message>
<xml_diff>
--- a/VT_REGION1_REF.xlsx
+++ b/VT_REGION1_REF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6B2AD8-FF79-48ED-BD19-13BBB5610ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468863CF-A6A6-410D-9954-15744A0F2E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -9468,6 +9468,24 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9497,24 +9515,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9552,31 +9552,10 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9595,6 +9574,27 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -18763,11 +18763,11 @@
   </sheetPr>
   <dimension ref="A1:BH117"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="F48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="8" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="O50" sqref="O50"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18975,150 +18975,150 @@
         <v>862</v>
       </c>
       <c r="V4" s="450" t="str">
-        <f>"AFA~UP~"&amp;V6</f>
-        <v>AFA~UP~2017</v>
+        <f>"AFA~FX~"&amp;V6</f>
+        <v>AFA~FX~2017</v>
       </c>
       <c r="W4" s="450" t="str">
-        <f t="shared" ref="W4:Z4" si="0">"AFA~UP~"&amp;W6</f>
-        <v>AFA~UP~2018</v>
+        <f t="shared" ref="W4:AC4" si="0">"AFA~FX~"&amp;W6</f>
+        <v>AFA~FX~2018</v>
       </c>
       <c r="X4" s="450" t="str">
         <f t="shared" si="0"/>
-        <v>AFA~UP~2019</v>
+        <v>AFA~FX~2019</v>
       </c>
       <c r="Y4" s="450" t="str">
         <f t="shared" si="0"/>
-        <v>AFA~UP~2020</v>
+        <v>AFA~FX~2020</v>
       </c>
       <c r="Z4" s="450" t="str">
         <f t="shared" si="0"/>
-        <v>AFA~UP~2021</v>
+        <v>AFA~FX~2021</v>
       </c>
       <c r="AA4" s="450" t="str">
-        <f t="shared" ref="AA4:AB4" si="1">"AFA~UP~"&amp;AA6</f>
-        <v>AFA~UP~2022</v>
+        <f t="shared" si="0"/>
+        <v>AFA~FX~2022</v>
       </c>
       <c r="AB4" s="450" t="str">
-        <f t="shared" si="1"/>
-        <v>AFA~UP~2023</v>
+        <f t="shared" si="0"/>
+        <v>AFA~FX~2023</v>
       </c>
       <c r="AC4" s="450" t="str">
-        <f t="shared" ref="AC4" si="2">"AFA~UP~"&amp;AC6</f>
-        <v>AFA~UP~2024</v>
+        <f t="shared" si="0"/>
+        <v>AFA~FX~2024</v>
       </c>
       <c r="AD4" s="451" t="s">
         <v>878</v>
       </c>
       <c r="AE4" s="449" t="str">
-        <f t="shared" ref="AE4:BF4" si="3">$AE$3&amp;"~"&amp;AE6</f>
+        <f t="shared" ref="AE4:BF4" si="1">$AE$3&amp;"~"&amp;AE6</f>
         <v>RESID~2017</v>
       </c>
       <c r="AF4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2018</v>
       </c>
       <c r="AG4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2019</v>
       </c>
       <c r="AH4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2020</v>
       </c>
       <c r="AI4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2021</v>
       </c>
       <c r="AJ4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2022</v>
       </c>
       <c r="AK4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2023</v>
       </c>
       <c r="AL4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2024</v>
       </c>
       <c r="AM4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2025</v>
       </c>
       <c r="AN4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2026</v>
       </c>
       <c r="AO4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2027</v>
       </c>
       <c r="AP4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2028</v>
       </c>
       <c r="AQ4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2029</v>
       </c>
       <c r="AR4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2030</v>
       </c>
       <c r="AS4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2031</v>
       </c>
       <c r="AT4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2032</v>
       </c>
       <c r="AU4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2033</v>
       </c>
       <c r="AV4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2034</v>
       </c>
       <c r="AW4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2035</v>
       </c>
       <c r="AX4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2036</v>
       </c>
       <c r="AY4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2037</v>
       </c>
       <c r="AZ4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2038</v>
       </c>
       <c r="BA4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2039</v>
       </c>
       <c r="BB4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2040</v>
       </c>
       <c r="BC4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2045</v>
       </c>
       <c r="BD4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2050</v>
       </c>
       <c r="BE4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2060</v>
       </c>
       <c r="BF4" s="449" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>RESID~2070</v>
       </c>
     </row>
@@ -19337,47 +19337,47 @@
         <v>2029</v>
       </c>
       <c r="AR6" s="459">
-        <f t="shared" ref="AR6:BB6" si="4">AQ6+1</f>
+        <f t="shared" ref="AR6:BB6" si="2">AQ6+1</f>
         <v>2030</v>
       </c>
       <c r="AS6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2031</v>
       </c>
       <c r="AT6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2032</v>
       </c>
       <c r="AU6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2033</v>
       </c>
       <c r="AV6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2034</v>
       </c>
       <c r="AW6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2035</v>
       </c>
       <c r="AX6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2036</v>
       </c>
       <c r="AY6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2037</v>
       </c>
       <c r="AZ6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2038</v>
       </c>
       <c r="BA6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2039</v>
       </c>
       <c r="BB6" s="459">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2040</v>
       </c>
       <c r="BC6" s="459">
@@ -19453,19 +19453,19 @@
         <v>0.76</v>
       </c>
       <c r="Z7" s="435">
-        <f t="shared" ref="Z7:AC7" si="5">Y7</f>
+        <f t="shared" ref="Z7:AC7" si="3">Y7</f>
         <v>0.76</v>
       </c>
       <c r="AA7" s="435">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
       <c r="AB7" s="435">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
       <c r="AC7" s="435">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
       <c r="AD7" s="464">
@@ -19744,7 +19744,7 @@
       <c r="AB11" s="436"/>
       <c r="AC11" s="436"/>
       <c r="AD11" s="435">
-        <f t="shared" ref="AD11:AD16" si="6">AD$7*F$7*H11</f>
+        <f t="shared" ref="AD11:AD16" si="4">AD$7*F$7*H11</f>
         <v>135.2943527381006</v>
       </c>
       <c r="AE11" s="465"/>
@@ -19813,7 +19813,7 @@
       <c r="AB12" s="436"/>
       <c r="AC12" s="436"/>
       <c r="AD12" s="435">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>119.014751183922</v>
       </c>
       <c r="AE12" s="465"/>
@@ -19882,7 +19882,7 @@
       <c r="AB13" s="436"/>
       <c r="AC13" s="436"/>
       <c r="AD13" s="435">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>98.912487042853513</v>
       </c>
       <c r="AE13" s="465"/>
@@ -19951,7 +19951,7 @@
       <c r="AB14" s="436"/>
       <c r="AC14" s="436"/>
       <c r="AD14" s="435">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>41.499520736419207</v>
       </c>
       <c r="AE14" s="465"/>
@@ -20020,7 +20020,7 @@
       <c r="AB15" s="436"/>
       <c r="AC15" s="436"/>
       <c r="AD15" s="435">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.0721455959640007</v>
       </c>
       <c r="AE15" s="465"/>
@@ -20089,7 +20089,7 @@
       <c r="AB16" s="436"/>
       <c r="AC16" s="436"/>
       <c r="AD16" s="435">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>17.814051090010466</v>
       </c>
       <c r="AE16" s="465"/>
@@ -20231,11 +20231,11 @@
         <v>0.76</v>
       </c>
       <c r="W18" s="435">
-        <f t="shared" ref="W18:X18" si="7">W7</f>
+        <f t="shared" ref="W18:X18" si="5">W7</f>
         <v>0.76</v>
       </c>
       <c r="X18" s="435">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.76</v>
       </c>
       <c r="Y18" s="435">
@@ -20528,7 +20528,7 @@
       <c r="AB22" s="436"/>
       <c r="AC22" s="436"/>
       <c r="AD22" s="435">
-        <f t="shared" ref="AD22:AD27" si="8">AD$18*F$18*H22</f>
+        <f t="shared" ref="AD22:AD27" si="6">AD$18*F$18*H22</f>
         <v>50.96390846852993</v>
       </c>
       <c r="AE22" s="465"/>
@@ -20598,7 +20598,7 @@
       <c r="AB23" s="436"/>
       <c r="AC23" s="436"/>
       <c r="AD23" s="435">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>43.372266387120007</v>
       </c>
       <c r="AE23" s="465"/>
@@ -20668,7 +20668,7 @@
       <c r="AB24" s="436"/>
       <c r="AC24" s="436"/>
       <c r="AD24" s="435">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>29.179342140453457</v>
       </c>
       <c r="AE24" s="465"/>
@@ -20738,7 +20738,7 @@
       <c r="AB25" s="436"/>
       <c r="AC25" s="436"/>
       <c r="AD25" s="435">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>18.093933000670802</v>
       </c>
       <c r="AE25" s="465"/>
@@ -20808,7 +20808,7 @@
       <c r="AB26" s="436"/>
       <c r="AC26" s="436"/>
       <c r="AD26" s="435">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.8409817404492801</v>
       </c>
       <c r="AE26" s="465"/>
@@ -20878,7 +20878,7 @@
       <c r="AB27" s="436"/>
       <c r="AC27" s="436"/>
       <c r="AD27" s="435">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.8586058666101857</v>
       </c>
       <c r="AE27" s="465"/>
@@ -21020,11 +21020,11 @@
         <v>0.76</v>
       </c>
       <c r="W29" s="442">
-        <f t="shared" ref="W29:X29" si="9">W18</f>
+        <f t="shared" ref="W29:X29" si="7">W18</f>
         <v>0.76</v>
       </c>
       <c r="X29" s="442">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.76</v>
       </c>
       <c r="Y29" s="442">
@@ -21035,7 +21035,7 @@
         <v>0.76</v>
       </c>
       <c r="AA29" s="442">
-        <f t="shared" ref="AA29" si="10">X29</f>
+        <f t="shared" ref="AA29" si="8">X29</f>
         <v>0.76</v>
       </c>
       <c r="AB29" s="442">
@@ -21323,7 +21323,7 @@
       <c r="AB33" s="436"/>
       <c r="AC33" s="436"/>
       <c r="AD33" s="435">
-        <f t="shared" ref="AD33:AD38" si="11">AD$29*F$29*H33</f>
+        <f t="shared" ref="AD33:AD38" si="9">AD$29*F$29*H33</f>
         <v>62.108753503321424</v>
       </c>
       <c r="AE33" s="465"/>
@@ -21393,7 +21393,7 @@
       <c r="AB34" s="436"/>
       <c r="AC34" s="436"/>
       <c r="AD34" s="435">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>52.224285451851813</v>
       </c>
       <c r="AE34" s="465"/>
@@ -21463,7 +21463,7 @@
       <c r="AB35" s="436"/>
       <c r="AC35" s="436"/>
       <c r="AD35" s="435">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.9751176860345625</v>
       </c>
       <c r="AE35" s="465"/>
@@ -21533,7 +21533,7 @@
       <c r="AB36" s="436"/>
       <c r="AC36" s="436"/>
       <c r="AD36" s="435">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>34.464758096160011</v>
       </c>
       <c r="AE36" s="465"/>
@@ -21603,7 +21603,7 @@
       <c r="AB37" s="436"/>
       <c r="AC37" s="436"/>
       <c r="AD37" s="435">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0.42767644284377521</v>
       </c>
       <c r="AE37" s="465"/>
@@ -21673,7 +21673,7 @@
       <c r="AB38" s="436"/>
       <c r="AC38" s="436"/>
       <c r="AD38" s="435">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6.0408502943351339</v>
       </c>
       <c r="AE38" s="465"/>
@@ -22025,7 +22025,7 @@
       <c r="AB43" s="436"/>
       <c r="AC43" s="436"/>
       <c r="AD43" s="435">
-        <f t="shared" ref="AD43:AD48" si="12">AD$40*F$40*H43</f>
+        <f t="shared" ref="AD43:AD48" si="10">AD$40*F$40*H43</f>
         <v>1.0986365425199789</v>
       </c>
       <c r="AE43" s="465"/>
@@ -22093,7 +22093,7 @@
       <c r="AB44" s="436"/>
       <c r="AC44" s="436"/>
       <c r="AD44" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.6479548137799682</v>
       </c>
       <c r="AE44" s="465"/>
@@ -22161,7 +22161,7 @@
       <c r="AB45" s="436"/>
       <c r="AC45" s="436"/>
       <c r="AD45" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>14.55693418838972</v>
       </c>
       <c r="AE45" s="465"/>
@@ -22229,7 +22229,7 @@
       <c r="AB46" s="436"/>
       <c r="AC46" s="436"/>
       <c r="AD46" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>3.0212504919299419</v>
       </c>
       <c r="AE46" s="465"/>
@@ -22297,7 +22297,7 @@
       <c r="AB47" s="436"/>
       <c r="AC47" s="436"/>
       <c r="AD47" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2.1972730850399578</v>
       </c>
       <c r="AE47" s="465"/>
@@ -22365,7 +22365,7 @@
       <c r="AB48" s="436"/>
       <c r="AC48" s="436"/>
       <c r="AD48" s="435">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4.9438644413399047</v>
       </c>
       <c r="AE48" s="465"/>
@@ -24220,7 +24220,7 @@
       <c r="AB75" s="436"/>
       <c r="AC75" s="436"/>
       <c r="AD75" s="435">
-        <f t="shared" ref="AD75:AD80" si="13">AD$70*F$70*H75</f>
+        <f t="shared" ref="AD75:AD80" si="11">AD$70*F$70*H75</f>
         <v>53.084026088903464</v>
       </c>
       <c r="AE75" s="465"/>
@@ -24290,7 +24290,7 @@
       <c r="AB76" s="436"/>
       <c r="AC76" s="436"/>
       <c r="AD76" s="435">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>120.52809004075719</v>
       </c>
       <c r="AE76" s="465"/>
@@ -24360,7 +24360,7 @@
       <c r="AB77" s="436"/>
       <c r="AC77" s="436"/>
       <c r="AD77" s="435">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5.9468278391547447</v>
       </c>
       <c r="AE77" s="465"/>
@@ -24430,7 +24430,7 @@
       <c r="AB78" s="436"/>
       <c r="AC78" s="436"/>
       <c r="AD78" s="435">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>9.6672857142857165</v>
       </c>
       <c r="AE78" s="465"/>
@@ -24500,7 +24500,7 @@
       <c r="AB79" s="436"/>
       <c r="AC79" s="436"/>
       <c r="AD79" s="435">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3.0670273988922867</v>
       </c>
       <c r="AE79" s="465"/>
@@ -24570,7 +24570,7 @@
       <c r="AB80" s="436"/>
       <c r="AC80" s="436"/>
       <c r="AD80" s="435">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>20.5262472791314</v>
       </c>
       <c r="AE80" s="465"/>
@@ -26487,7 +26487,7 @@
         <v>499</v>
       </c>
       <c r="AD112" s="117">
-        <f t="shared" ref="AD112:AD117" si="14">SUMIF($E$7:$E$107,E112,$AD$7:$AD$107)</f>
+        <f t="shared" ref="AD112:AD117" si="12">SUMIF($E$7:$E$107,E112,$AD$7:$AD$107)</f>
         <v>303.09899561263535</v>
       </c>
     </row>
@@ -26496,7 +26496,7 @@
         <v>497</v>
       </c>
       <c r="AD113" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>349.69632725204076</v>
       </c>
     </row>
@@ -26505,7 +26505,7 @@
         <v>491</v>
       </c>
       <c r="AD114" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>135.16558341186152</v>
       </c>
     </row>
@@ -26514,7 +26514,7 @@
         <v>490</v>
       </c>
       <c r="AD115" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>106.74674803946569</v>
       </c>
     </row>
@@ -26523,7 +26523,7 @@
         <v>487</v>
       </c>
       <c r="AD116" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>16.6051042631893</v>
       </c>
     </row>
@@ -26532,7 +26532,7 @@
         <v>485</v>
       </c>
       <c r="AD117" s="117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>52.183618971427094</v>
       </c>
     </row>
@@ -26550,7 +26550,7 @@
   </sheetPr>
   <dimension ref="A1:AH286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+    <sheetView topLeftCell="A237" workbookViewId="0">
       <selection activeCell="N267" sqref="N267"/>
     </sheetView>
   </sheetViews>
@@ -34453,26 +34453,26 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="96" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="496" t="s">
+      <c r="C2" s="486" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="497"/>
-      <c r="E2" s="497"/>
-      <c r="F2" s="498" t="s">
+      <c r="D2" s="487"/>
+      <c r="E2" s="487"/>
+      <c r="F2" s="488" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="499"/>
-      <c r="H2" s="500"/>
-      <c r="I2" s="498" t="s">
+      <c r="G2" s="489"/>
+      <c r="H2" s="490"/>
+      <c r="I2" s="488" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="499"/>
-      <c r="K2" s="500"/>
-      <c r="L2" s="498" t="s">
+      <c r="J2" s="489"/>
+      <c r="K2" s="490"/>
+      <c r="L2" s="488" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="499"/>
-      <c r="N2" s="500"/>
+      <c r="M2" s="489"/>
+      <c r="N2" s="490"/>
       <c r="O2" s="97"/>
       <c r="P2" s="13"/>
       <c r="AA2" s="96" t="s">
@@ -34745,10 +34745,10 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="485" t="s">
+      <c r="A9" s="491" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="486"/>
+      <c r="B9" s="492"/>
       <c r="C9" s="49"/>
       <c r="D9" s="44">
         <f>D5/$O$5</f>
@@ -34773,49 +34773,49 @@
       <c r="O9" s="7">
         <v>788</v>
       </c>
-      <c r="Q9" s="491" t="s">
+      <c r="Q9" s="497" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="493" t="s">
+      <c r="S9" s="499" t="s">
         <v>83</v>
       </c>
-      <c r="V9" s="489" t="s">
+      <c r="V9" s="495" t="s">
         <v>881</v>
       </c>
-      <c r="W9" s="489" t="s">
+      <c r="W9" s="495" t="s">
         <v>882</v>
       </c>
-      <c r="X9" s="489" t="s">
+      <c r="X9" s="495" t="s">
         <v>82</v>
       </c>
-      <c r="Y9" s="489" t="s">
+      <c r="Y9" s="495" t="s">
         <v>883</v>
       </c>
-      <c r="Z9" s="489" t="s">
+      <c r="Z9" s="495" t="s">
         <v>884</v>
       </c>
-      <c r="AA9" s="489" t="s">
+      <c r="AA9" s="495" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="489" t="s">
+      <c r="AB9" s="495" t="s">
         <v>885</v>
       </c>
-      <c r="AC9" s="489" t="s">
+      <c r="AC9" s="495" t="s">
         <v>886</v>
       </c>
-      <c r="AD9" s="489" t="s">
+      <c r="AD9" s="495" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="489" t="s">
+      <c r="AE9" s="495" t="s">
         <v>887</v>
       </c>
-      <c r="AF9" s="489" t="s">
+      <c r="AF9" s="495" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="487"/>
-      <c r="B10" s="488"/>
+      <c r="A10" s="493"/>
+      <c r="B10" s="494"/>
       <c r="C10" s="49"/>
       <c r="D10" s="9">
         <f>D9*788</f>
@@ -34841,25 +34841,25 @@
         <f>O9-G10</f>
         <v>422.2729198252656</v>
       </c>
-      <c r="Q10" s="492"/>
+      <c r="Q10" s="498"/>
       <c r="R10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="S10" s="494"/>
+      <c r="S10" s="500"/>
       <c r="U10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="V10" s="490"/>
-      <c r="W10" s="490"/>
-      <c r="X10" s="490"/>
-      <c r="Y10" s="490"/>
-      <c r="Z10" s="490"/>
-      <c r="AA10" s="490"/>
-      <c r="AB10" s="490"/>
-      <c r="AC10" s="490"/>
-      <c r="AD10" s="490"/>
-      <c r="AE10" s="490"/>
-      <c r="AF10" s="490"/>
+      <c r="V10" s="496"/>
+      <c r="W10" s="496"/>
+      <c r="X10" s="496"/>
+      <c r="Y10" s="496"/>
+      <c r="Z10" s="496"/>
+      <c r="AA10" s="496"/>
+      <c r="AB10" s="496"/>
+      <c r="AC10" s="496"/>
+      <c r="AD10" s="496"/>
+      <c r="AE10" s="496"/>
+      <c r="AF10" s="496"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
@@ -37351,11 +37351,11 @@
       <c r="J62" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="495" t="s">
+      <c r="K62" s="485" t="s">
         <v>26</v>
       </c>
-      <c r="L62" s="495"/>
-      <c r="M62" s="495"/>
+      <c r="L62" s="485"/>
+      <c r="M62" s="485"/>
       <c r="N62"/>
     </row>
     <row r="63" spans="3:22" ht="15" x14ac:dyDescent="0.25">
@@ -37613,11 +37613,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AC9:AC10"/>
@@ -37632,6 +37627,11 @@
     <mergeCell ref="AB9:AB10"/>
     <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="W9:W10"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40300,7 +40300,7 @@
         <v>190</v>
       </c>
       <c r="G2" s="509"/>
-      <c r="H2" s="500"/>
+      <c r="H2" s="490"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -40542,7 +40542,7 @@
       <c r="G14" s="88"/>
       <c r="H14" s="154"/>
       <c r="I14" s="153"/>
-      <c r="J14" s="494"/>
+      <c r="J14" s="500"/>
       <c r="K14" s="152" t="s">
         <v>79</v>
       </c>
@@ -44430,27 +44430,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="521" t="s">
+      <c r="A1" s="513" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="516"/>
-      <c r="C1" s="516"/>
-      <c r="D1" s="516"/>
-      <c r="E1" s="516"/>
-      <c r="F1" s="516"/>
-      <c r="G1" s="516"/>
-      <c r="H1" s="516"/>
-      <c r="I1" s="516"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
       <c r="J1" s="216" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="522" t="s">
+      <c r="A2" s="515" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
+      <c r="B2" s="515"/>
+      <c r="C2" s="515"/>
       <c r="D2" s="259">
         <v>2019</v>
       </c>
@@ -44487,16 +44487,16 @@
       <c r="U2" s="252"/>
     </row>
     <row r="3" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="523" t="s">
+      <c r="A3" s="516" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="523"/>
+      <c r="B3" s="516"/>
       <c r="C3" s="254"/>
       <c r="D3" s="255"/>
       <c r="E3" s="254"/>
       <c r="F3" s="254"/>
       <c r="G3" s="253"/>
-      <c r="H3" s="524" t="s">
+      <c r="H3" s="517" t="s">
         <v>373</v>
       </c>
       <c r="Q3"/>
@@ -44506,10 +44506,10 @@
       <c r="U3" s="252"/>
     </row>
     <row r="4" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="527" t="s">
+      <c r="A4" s="520" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="527"/>
+      <c r="B4" s="520"/>
       <c r="C4" s="241">
         <v>1</v>
       </c>
@@ -44525,7 +44525,7 @@
       <c r="G4" s="221">
         <v>18806</v>
       </c>
-      <c r="H4" s="525"/>
+      <c r="H4" s="518"/>
       <c r="J4" s="216">
         <f>D4/F4</f>
         <v>0.99859246427024684</v>
@@ -44543,10 +44543,10 @@
       <c r="T4" s="252"/>
     </row>
     <row r="5" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="513" t="s">
+      <c r="A5" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="513"/>
+      <c r="B5" s="521"/>
       <c r="C5" s="239"/>
       <c r="D5" s="231">
         <v>6736</v>
@@ -44560,13 +44560,13 @@
       <c r="G5" s="221">
         <v>7019</v>
       </c>
-      <c r="H5" s="525"/>
+      <c r="H5" s="518"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="513" t="s">
+      <c r="A6" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="513"/>
+      <c r="B6" s="521"/>
       <c r="C6" s="239"/>
       <c r="D6" s="231">
         <v>1467</v>
@@ -44580,13 +44580,13 @@
       <c r="G6" s="221">
         <v>1461</v>
       </c>
-      <c r="H6" s="525"/>
+      <c r="H6" s="518"/>
     </row>
     <row r="7" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="513" t="s">
+      <c r="A7" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="513"/>
+      <c r="B7" s="521"/>
       <c r="C7" s="239"/>
       <c r="D7" s="231">
         <v>3209</v>
@@ -44600,13 +44600,13 @@
       <c r="G7" s="221">
         <v>3331</v>
       </c>
-      <c r="H7" s="525"/>
+      <c r="H7" s="518"/>
     </row>
     <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="513" t="s">
+      <c r="A8" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B8" s="513"/>
+      <c r="B8" s="521"/>
       <c r="C8" s="239"/>
       <c r="D8" s="231">
         <v>4271</v>
@@ -44620,13 +44620,13 @@
       <c r="G8" s="221">
         <v>4067</v>
       </c>
-      <c r="H8" s="525"/>
+      <c r="H8" s="518"/>
     </row>
     <row r="9" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="513" t="s">
+      <c r="A9" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="513"/>
+      <c r="B9" s="521"/>
       <c r="C9" s="239"/>
       <c r="D9" s="231">
         <v>1277</v>
@@ -44640,13 +44640,13 @@
       <c r="G9" s="221">
         <v>1309</v>
       </c>
-      <c r="H9" s="525"/>
+      <c r="H9" s="518"/>
     </row>
     <row r="10" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="513" t="s">
+      <c r="A10" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="513"/>
+      <c r="B10" s="521"/>
       <c r="C10" s="239"/>
       <c r="D10" s="233">
         <v>688</v>
@@ -44660,13 +44660,13 @@
       <c r="G10" s="218">
         <v>793</v>
       </c>
-      <c r="H10" s="525"/>
+      <c r="H10" s="518"/>
     </row>
     <row r="11" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="513" t="s">
+      <c r="A11" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="513"/>
+      <c r="B11" s="521"/>
       <c r="C11" s="239"/>
       <c r="D11" s="233">
         <v>53</v>
@@ -44680,14 +44680,14 @@
       <c r="G11" s="218">
         <v>62</v>
       </c>
-      <c r="H11" s="525"/>
+      <c r="H11" s="518"/>
     </row>
     <row r="12" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="514" t="s">
+      <c r="A12" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B12" s="514"/>
-      <c r="C12" s="514"/>
+      <c r="B12" s="522"/>
+      <c r="C12" s="522"/>
       <c r="D12" s="251">
         <v>745</v>
       </c>
@@ -44700,14 +44700,14 @@
       <c r="G12" s="249">
         <v>763</v>
       </c>
-      <c r="H12" s="526"/>
+      <c r="H12" s="519"/>
       <c r="V12" s="243"/>
     </row>
     <row r="13" spans="1:22" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="520" t="s">
+      <c r="A13" s="523" t="s">
         <v>396</v>
       </c>
-      <c r="B13" s="520"/>
+      <c r="B13" s="523"/>
       <c r="C13" s="248">
         <v>2</v>
       </c>
@@ -44719,10 +44719,10 @@
       <c r="V13" s="243"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="516" t="s">
+      <c r="A14" s="514" t="s">
         <v>395</v>
       </c>
-      <c r="B14" s="516"/>
+      <c r="B14" s="514"/>
       <c r="C14" s="239"/>
       <c r="D14" s="231">
         <v>105.04</v>
@@ -44757,10 +44757,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="513" t="s">
+      <c r="A15" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="513"/>
+      <c r="B15" s="521"/>
       <c r="C15" s="239"/>
       <c r="D15" s="231">
         <v>96.16</v>
@@ -44793,10 +44793,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="513" t="s">
+      <c r="A16" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="513"/>
+      <c r="B16" s="521"/>
       <c r="C16" s="239"/>
       <c r="D16" s="231">
         <v>5.34</v>
@@ -44829,10 +44829,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="513" t="s">
+      <c r="A17" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B17" s="513"/>
+      <c r="B17" s="521"/>
       <c r="C17" s="239"/>
       <c r="D17" s="231">
         <v>3.49</v>
@@ -44865,10 +44865,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="513" t="s">
+      <c r="A18" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B18" s="513"/>
+      <c r="B18" s="521"/>
       <c r="C18" s="239"/>
       <c r="D18" s="242">
         <v>0</v>
@@ -44901,10 +44901,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="513" t="s">
+      <c r="A19" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="513"/>
+      <c r="B19" s="521"/>
       <c r="C19" s="239"/>
       <c r="D19" s="231">
         <v>0</v>
@@ -44937,10 +44937,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="513" t="s">
+      <c r="A20" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B20" s="513"/>
+      <c r="B20" s="521"/>
       <c r="C20" s="239"/>
       <c r="D20" s="231">
         <v>0.04</v>
@@ -44973,10 +44973,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="513" t="s">
+      <c r="A21" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B21" s="513"/>
+      <c r="B21" s="521"/>
       <c r="C21" s="239"/>
       <c r="D21" s="231">
         <v>0</v>
@@ -45009,11 +45009,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="513" t="s">
+      <c r="A22" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B22" s="513"/>
-      <c r="C22" s="513"/>
+      <c r="B22" s="521"/>
+      <c r="C22" s="521"/>
       <c r="D22" s="231">
         <v>0.01</v>
       </c>
@@ -45045,10 +45045,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="516" t="s">
+      <c r="A23" s="514" t="s">
         <v>394</v>
       </c>
-      <c r="B23" s="516"/>
+      <c r="B23" s="514"/>
       <c r="C23" s="239"/>
       <c r="D23" s="231">
         <v>1.64</v>
@@ -45083,10 +45083,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="513" t="s">
+      <c r="A24" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B24" s="513"/>
+      <c r="B24" s="521"/>
       <c r="C24" s="239"/>
       <c r="D24" s="231">
         <v>0.9</v>
@@ -45119,10 +45119,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="513" t="s">
+      <c r="A25" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="513"/>
+      <c r="B25" s="521"/>
       <c r="C25" s="239"/>
       <c r="D25" s="231">
         <v>0.73</v>
@@ -45155,10 +45155,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="513" t="s">
+      <c r="A26" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B26" s="513"/>
+      <c r="B26" s="521"/>
       <c r="C26" s="239"/>
       <c r="D26" s="231">
         <v>0</v>
@@ -45191,10 +45191,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="513" t="s">
+      <c r="A27" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B27" s="513"/>
+      <c r="B27" s="521"/>
       <c r="C27" s="239"/>
       <c r="D27" s="231">
         <v>0</v>
@@ -45227,10 +45227,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="513" t="s">
+      <c r="A28" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="513"/>
+      <c r="B28" s="521"/>
       <c r="C28" s="239"/>
       <c r="D28" s="231">
         <v>0</v>
@@ -45263,10 +45263,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="513" t="s">
+      <c r="A29" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B29" s="513"/>
+      <c r="B29" s="521"/>
       <c r="C29" s="239"/>
       <c r="D29" s="231">
         <v>0.01</v>
@@ -45299,10 +45299,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="513" t="s">
+      <c r="A30" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B30" s="513"/>
+      <c r="B30" s="521"/>
       <c r="C30" s="239"/>
       <c r="D30" s="231">
         <v>0</v>
@@ -45335,11 +45335,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="513" t="s">
+      <c r="A31" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B31" s="513"/>
-      <c r="C31" s="513"/>
+      <c r="B31" s="521"/>
+      <c r="C31" s="521"/>
       <c r="D31" s="231">
         <v>0</v>
       </c>
@@ -45371,10 +45371,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="516" t="s">
+      <c r="A32" s="514" t="s">
         <v>393</v>
       </c>
-      <c r="B32" s="516"/>
+      <c r="B32" s="514"/>
       <c r="C32" s="239"/>
       <c r="D32" s="231">
         <v>56004</v>
@@ -45409,10 +45409,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="513" t="s">
+      <c r="A33" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B33" s="513"/>
+      <c r="B33" s="521"/>
       <c r="C33" s="239"/>
       <c r="D33" s="231">
         <v>48418</v>
@@ -45451,10 +45451,10 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="513" t="s">
+      <c r="A34" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="513"/>
+      <c r="B34" s="521"/>
       <c r="C34" s="239"/>
       <c r="D34" s="231">
         <v>4557</v>
@@ -45487,10 +45487,10 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="513" t="s">
+      <c r="A35" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B35" s="513"/>
+      <c r="B35" s="521"/>
       <c r="C35" s="239"/>
       <c r="D35" s="233">
         <v>16</v>
@@ -45523,10 +45523,10 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="513" t="s">
+      <c r="A36" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B36" s="513"/>
+      <c r="B36" s="521"/>
       <c r="C36" s="239"/>
       <c r="D36" s="233">
         <v>932</v>
@@ -45559,10 +45559,10 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="513" t="s">
+      <c r="A37" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B37" s="513"/>
+      <c r="B37" s="521"/>
       <c r="C37" s="239"/>
       <c r="D37" s="233">
         <v>610</v>
@@ -45595,10 +45595,10 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="513" t="s">
+      <c r="A38" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="513"/>
+      <c r="B38" s="521"/>
       <c r="C38" s="239"/>
       <c r="D38" s="231">
         <v>1163</v>
@@ -45631,10 +45631,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="513" t="s">
+      <c r="A39" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B39" s="513"/>
+      <c r="B39" s="521"/>
       <c r="C39" s="239"/>
       <c r="D39" s="233">
         <v>261</v>
@@ -45667,11 +45667,11 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="513" t="s">
+      <c r="A40" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B40" s="513"/>
-      <c r="C40" s="513"/>
+      <c r="B40" s="521"/>
+      <c r="C40" s="521"/>
       <c r="D40" s="233">
         <v>47</v>
       </c>
@@ -45703,10 +45703,10 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="516" t="s">
+      <c r="A41" s="514" t="s">
         <v>391</v>
       </c>
-      <c r="B41" s="516"/>
+      <c r="B41" s="514"/>
       <c r="C41" s="241">
         <v>3</v>
       </c>
@@ -45727,10 +45727,10 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="513" t="s">
+      <c r="A42" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B42" s="513"/>
+      <c r="B42" s="521"/>
       <c r="C42" s="239"/>
       <c r="D42" s="231">
         <v>5596</v>
@@ -45766,10 +45766,10 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="513" t="s">
+      <c r="A43" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="513"/>
+      <c r="B43" s="521"/>
       <c r="C43" s="239"/>
       <c r="D43" s="233">
         <v>400</v>
@@ -45805,10 +45805,10 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="513" t="s">
+      <c r="A44" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B44" s="513"/>
+      <c r="B44" s="521"/>
       <c r="C44" s="239"/>
       <c r="D44" s="233">
         <v>726</v>
@@ -45844,10 +45844,10 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="513" t="s">
+      <c r="A45" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="513"/>
+      <c r="B45" s="521"/>
       <c r="C45" s="239"/>
       <c r="D45" s="233">
         <v>289</v>
@@ -45883,10 +45883,10 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="513" t="s">
+      <c r="A46" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B46" s="513"/>
+      <c r="B46" s="521"/>
       <c r="C46" s="239"/>
       <c r="D46" s="233">
         <v>108</v>
@@ -45903,10 +45903,10 @@
       <c r="H46" s="230"/>
     </row>
     <row r="47" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="513" t="s">
+      <c r="A47" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="513"/>
+      <c r="B47" s="521"/>
       <c r="C47" s="239"/>
       <c r="D47" s="233">
         <v>498</v>
@@ -45923,10 +45923,10 @@
       <c r="H47" s="230"/>
     </row>
     <row r="48" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="513" t="s">
+      <c r="A48" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="513"/>
+      <c r="B48" s="521"/>
       <c r="C48" s="239"/>
       <c r="D48" s="231">
         <v>0</v>
@@ -45943,11 +45943,11 @@
       <c r="H48" s="230"/>
     </row>
     <row r="49" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="513" t="s">
+      <c r="A49" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="513"/>
-      <c r="C49" s="513"/>
+      <c r="B49" s="521"/>
+      <c r="C49" s="521"/>
       <c r="D49" s="233">
         <v>36</v>
       </c>
@@ -45963,10 +45963,10 @@
       <c r="H49" s="230"/>
     </row>
     <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="516" t="s">
+      <c r="A50" s="514" t="s">
         <v>390</v>
       </c>
-      <c r="B50" s="516"/>
+      <c r="B50" s="514"/>
       <c r="C50" s="241">
         <v>4</v>
       </c>
@@ -45987,10 +45987,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="513" t="s">
+      <c r="A51" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B51" s="513"/>
+      <c r="B51" s="521"/>
       <c r="C51" s="239"/>
       <c r="D51" s="231">
         <v>0</v>
@@ -46007,10 +46007,10 @@
       <c r="H51" s="230"/>
     </row>
     <row r="52" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="513" t="s">
+      <c r="A52" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B52" s="513"/>
+      <c r="B52" s="521"/>
       <c r="C52" s="239"/>
       <c r="D52" s="231">
         <v>0</v>
@@ -46027,10 +46027,10 @@
       <c r="H52" s="230"/>
     </row>
     <row r="53" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="513" t="s">
+      <c r="A53" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B53" s="513"/>
+      <c r="B53" s="521"/>
       <c r="C53" s="239"/>
       <c r="D53" s="231">
         <v>0</v>
@@ -46047,10 +46047,10 @@
       <c r="H53" s="230"/>
     </row>
     <row r="54" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="513" t="s">
+      <c r="A54" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B54" s="513"/>
+      <c r="B54" s="521"/>
       <c r="C54" s="239"/>
       <c r="D54" s="231">
         <v>0</v>
@@ -46067,10 +46067,10 @@
       <c r="H54" s="230"/>
     </row>
     <row r="55" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="513" t="s">
+      <c r="A55" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B55" s="513"/>
+      <c r="B55" s="521"/>
       <c r="C55" s="239"/>
       <c r="D55" s="231">
         <v>0</v>
@@ -46087,10 +46087,10 @@
       <c r="H55" s="230"/>
     </row>
     <row r="56" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="513" t="s">
+      <c r="A56" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B56" s="513"/>
+      <c r="B56" s="521"/>
       <c r="C56" s="239"/>
       <c r="D56" s="231">
         <v>0</v>
@@ -46107,10 +46107,10 @@
       <c r="H56" s="230"/>
     </row>
     <row r="57" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="513" t="s">
+      <c r="A57" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="513"/>
+      <c r="B57" s="521"/>
       <c r="C57" s="239"/>
       <c r="D57" s="231">
         <v>0.05</v>
@@ -46127,11 +46127,11 @@
       <c r="H57" s="230"/>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="514" t="s">
+      <c r="A58" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B58" s="514"/>
-      <c r="C58" s="514"/>
+      <c r="B58" s="522"/>
+      <c r="C58" s="522"/>
       <c r="D58" s="229">
         <v>0</v>
       </c>
@@ -46147,46 +46147,46 @@
       <c r="H58" s="238"/>
     </row>
     <row r="59" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="516"/>
-      <c r="B59" s="516"/>
-      <c r="C59" s="516"/>
-      <c r="D59" s="516"/>
-      <c r="E59" s="516"/>
-      <c r="F59" s="516"/>
-      <c r="G59" s="516"/>
-      <c r="H59" s="516"/>
-      <c r="I59" s="516"/>
+      <c r="A59" s="514"/>
+      <c r="B59" s="514"/>
+      <c r="C59" s="514"/>
+      <c r="D59" s="514"/>
+      <c r="E59" s="514"/>
+      <c r="F59" s="514"/>
+      <c r="G59" s="514"/>
+      <c r="H59" s="514"/>
+      <c r="I59" s="514"/>
     </row>
     <row r="60" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="516"/>
-      <c r="B60" s="516"/>
-      <c r="C60" s="516"/>
-      <c r="D60" s="516"/>
-      <c r="E60" s="516"/>
-      <c r="F60" s="516"/>
-      <c r="G60" s="516"/>
-      <c r="H60" s="516"/>
-      <c r="I60" s="516"/>
+      <c r="A60" s="514"/>
+      <c r="B60" s="514"/>
+      <c r="C60" s="514"/>
+      <c r="D60" s="514"/>
+      <c r="E60" s="514"/>
+      <c r="F60" s="514"/>
+      <c r="G60" s="514"/>
+      <c r="H60" s="514"/>
+      <c r="I60" s="514"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="519" t="s">
+      <c r="A61" s="524" t="s">
         <v>388</v>
       </c>
-      <c r="B61" s="519"/>
-      <c r="C61" s="519"/>
-      <c r="D61" s="519"/>
-      <c r="E61" s="519"/>
-      <c r="F61" s="519"/>
-      <c r="G61" s="519"/>
-      <c r="H61" s="519"/>
-      <c r="I61" s="519"/>
+      <c r="B61" s="524"/>
+      <c r="C61" s="524"/>
+      <c r="D61" s="524"/>
+      <c r="E61" s="524"/>
+      <c r="F61" s="524"/>
+      <c r="G61" s="524"/>
+      <c r="H61" s="524"/>
+      <c r="I61" s="524"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="517" t="s">
+      <c r="A62" s="525" t="s">
         <v>345</v>
       </c>
-      <c r="B62" s="517"/>
-      <c r="C62" s="517"/>
+      <c r="B62" s="525"/>
+      <c r="C62" s="525"/>
       <c r="D62" s="225">
         <v>2019</v>
       </c>
@@ -46204,11 +46204,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="518" t="s">
+      <c r="A63" s="526" t="s">
         <v>344</v>
       </c>
-      <c r="B63" s="518"/>
-      <c r="C63" s="518"/>
+      <c r="B63" s="526"/>
+      <c r="C63" s="526"/>
       <c r="D63" s="220" t="s">
         <v>386</v>
       </c>
@@ -46226,11 +46226,11 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="513" t="s">
+      <c r="A64" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="513"/>
-      <c r="C64" s="513"/>
+      <c r="B64" s="521"/>
+      <c r="C64" s="521"/>
       <c r="D64" s="231" t="s">
         <v>382</v>
       </c>
@@ -46246,11 +46246,11 @@
       <c r="H64" s="230"/>
     </row>
     <row r="65" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="513" t="s">
+      <c r="A65" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B65" s="513"/>
-      <c r="C65" s="513"/>
+      <c r="B65" s="521"/>
+      <c r="C65" s="521"/>
       <c r="D65" s="231" t="s">
         <v>380</v>
       </c>
@@ -46266,11 +46266,11 @@
       <c r="H65" s="230"/>
     </row>
     <row r="66" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="513" t="s">
+      <c r="A66" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B66" s="513"/>
-      <c r="C66" s="513"/>
+      <c r="B66" s="521"/>
+      <c r="C66" s="521"/>
       <c r="D66" s="233">
         <v>822</v>
       </c>
@@ -46286,11 +46286,11 @@
       <c r="H66" s="230"/>
     </row>
     <row r="67" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="513" t="s">
+      <c r="A67" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B67" s="513"/>
-      <c r="C67" s="513"/>
+      <c r="B67" s="521"/>
+      <c r="C67" s="521"/>
       <c r="D67" s="231" t="s">
         <v>379</v>
       </c>
@@ -46306,11 +46306,11 @@
       <c r="H67" s="230"/>
     </row>
     <row r="68" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="513" t="s">
+      <c r="A68" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="513"/>
-      <c r="C68" s="513"/>
+      <c r="B68" s="521"/>
+      <c r="C68" s="521"/>
       <c r="D68" s="233">
         <v>717</v>
       </c>
@@ -46326,11 +46326,11 @@
       <c r="H68" s="230"/>
     </row>
     <row r="69" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="513" t="s">
+      <c r="A69" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="513"/>
-      <c r="C69" s="513"/>
+      <c r="B69" s="521"/>
+      <c r="C69" s="521"/>
       <c r="D69" s="231" t="s">
         <v>378</v>
       </c>
@@ -46346,11 +46346,11 @@
       <c r="H69" s="230"/>
     </row>
     <row r="70" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="513" t="s">
+      <c r="A70" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B70" s="513"/>
-      <c r="C70" s="513"/>
+      <c r="B70" s="521"/>
+      <c r="C70" s="521"/>
       <c r="D70" s="233">
         <v>261</v>
       </c>
@@ -46366,11 +46366,11 @@
       <c r="H70" s="230"/>
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="513" t="s">
+      <c r="A71" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B71" s="513"/>
-      <c r="C71" s="513"/>
+      <c r="B71" s="521"/>
+      <c r="C71" s="521"/>
       <c r="D71" s="233">
         <v>83</v>
       </c>
@@ -46386,11 +46386,11 @@
       <c r="H71" s="230"/>
     </row>
     <row r="72" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="516" t="s">
+      <c r="A72" s="514" t="s">
         <v>377</v>
       </c>
-      <c r="B72" s="516"/>
-      <c r="C72" s="516"/>
+      <c r="B72" s="514"/>
+      <c r="C72" s="514"/>
       <c r="D72" s="231" t="s">
         <v>368</v>
       </c>
@@ -46408,11 +46408,11 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="513" t="s">
+      <c r="A73" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B73" s="513"/>
-      <c r="C73" s="513"/>
+      <c r="B73" s="521"/>
+      <c r="C73" s="521"/>
       <c r="D73" s="231" t="s">
         <v>372</v>
       </c>
@@ -46428,11 +46428,11 @@
       <c r="H73" s="230"/>
     </row>
     <row r="74" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="513" t="s">
+      <c r="A74" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B74" s="513"/>
-      <c r="C74" s="513"/>
+      <c r="B74" s="521"/>
+      <c r="C74" s="521"/>
       <c r="D74" s="231" t="s">
         <v>368</v>
       </c>
@@ -46448,11 +46448,11 @@
       <c r="H74" s="230"/>
     </row>
     <row r="75" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="513" t="s">
+      <c r="A75" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B75" s="513"/>
-      <c r="C75" s="513"/>
+      <c r="B75" s="521"/>
+      <c r="C75" s="521"/>
       <c r="D75" s="231" t="s">
         <v>348</v>
       </c>
@@ -46468,11 +46468,11 @@
       <c r="H75" s="230"/>
     </row>
     <row r="76" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="513" t="s">
+      <c r="A76" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B76" s="513"/>
-      <c r="C76" s="513"/>
+      <c r="B76" s="521"/>
+      <c r="C76" s="521"/>
       <c r="D76" s="231" t="s">
         <v>362</v>
       </c>
@@ -46488,11 +46488,11 @@
       <c r="H76" s="230"/>
     </row>
     <row r="77" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="513" t="s">
+      <c r="A77" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B77" s="513"/>
-      <c r="C77" s="513"/>
+      <c r="B77" s="521"/>
+      <c r="C77" s="521"/>
       <c r="D77" s="231" t="s">
         <v>361</v>
       </c>
@@ -46508,11 +46508,11 @@
       <c r="H77" s="230"/>
     </row>
     <row r="78" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="513" t="s">
+      <c r="A78" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B78" s="513"/>
-      <c r="C78" s="513"/>
+      <c r="B78" s="521"/>
+      <c r="C78" s="521"/>
       <c r="D78" s="231" t="s">
         <v>358</v>
       </c>
@@ -46528,11 +46528,11 @@
       <c r="H78" s="230"/>
     </row>
     <row r="79" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="513" t="s">
+      <c r="A79" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="513"/>
-      <c r="C79" s="513"/>
+      <c r="B79" s="521"/>
+      <c r="C79" s="521"/>
       <c r="D79" s="231" t="s">
         <v>354</v>
       </c>
@@ -46548,11 +46548,11 @@
       <c r="H79" s="230"/>
     </row>
     <row r="80" spans="1:8" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="514" t="s">
+      <c r="A80" s="522" t="s">
         <v>324</v>
       </c>
-      <c r="B80" s="514"/>
-      <c r="C80" s="514"/>
+      <c r="B80" s="522"/>
+      <c r="C80" s="522"/>
       <c r="D80" s="229" t="s">
         <v>349</v>
       </c>
@@ -46568,30 +46568,30 @@
       <c r="H80" s="226"/>
     </row>
     <row r="81" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="515" t="s">
+      <c r="A81" s="527" t="s">
         <v>347</v>
       </c>
-      <c r="B81" s="516"/>
-      <c r="C81" s="516"/>
-      <c r="D81" s="516"/>
-      <c r="E81" s="516"/>
-      <c r="F81" s="516"/>
-      <c r="G81" s="516"/>
-      <c r="H81" s="516"/>
-      <c r="I81" s="516"/>
+      <c r="B81" s="514"/>
+      <c r="C81" s="514"/>
+      <c r="D81" s="514"/>
+      <c r="E81" s="514"/>
+      <c r="F81" s="514"/>
+      <c r="G81" s="514"/>
+      <c r="H81" s="514"/>
+      <c r="I81" s="514"/>
     </row>
     <row r="82" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="516" t="s">
+      <c r="A82" s="514" t="s">
         <v>346</v>
       </c>
-      <c r="B82" s="516"/>
-      <c r="C82" s="516"/>
-      <c r="D82" s="516"/>
-      <c r="E82" s="516"/>
-      <c r="F82" s="516"/>
-      <c r="G82" s="516"/>
-      <c r="H82" s="516"/>
-      <c r="I82" s="516"/>
+      <c r="B82" s="514"/>
+      <c r="C82" s="514"/>
+      <c r="D82" s="514"/>
+      <c r="E82" s="514"/>
+      <c r="F82" s="514"/>
+      <c r="G82" s="514"/>
+      <c r="H82" s="514"/>
+      <c r="I82" s="514"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D83" s="216" t="str">
@@ -46612,11 +46612,11 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="517" t="s">
+      <c r="A85" s="525" t="s">
         <v>345</v>
       </c>
-      <c r="B85" s="517"/>
-      <c r="C85" s="517"/>
+      <c r="B85" s="525"/>
+      <c r="C85" s="525"/>
       <c r="D85" s="225">
         <v>2019</v>
       </c>
@@ -46643,11 +46643,11 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="518" t="s">
+      <c r="A86" s="526" t="s">
         <v>344</v>
       </c>
-      <c r="B86" s="518"/>
-      <c r="C86" s="518"/>
+      <c r="B86" s="526"/>
+      <c r="C86" s="526"/>
       <c r="D86" s="220">
         <f>D14*gwpch4+D23*gwpn2o+D32+D41+D50</f>
         <v>66558.41</v>
@@ -46685,11 +46685,11 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="513" t="s">
+      <c r="A87" s="521" t="s">
         <v>340</v>
       </c>
-      <c r="B87" s="513"/>
-      <c r="C87" s="513"/>
+      <c r="B87" s="521"/>
+      <c r="C87" s="521"/>
       <c r="D87" s="220">
         <f t="shared" ref="D87:D94" si="14">D15*gwpch4+D24*gwpn2o+D33+D42+D51</f>
         <v>56492.08</v>
@@ -46724,11 +46724,11 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="513" t="s">
+      <c r="A88" s="521" t="s">
         <v>336</v>
       </c>
-      <c r="B88" s="513"/>
-      <c r="C88" s="513"/>
+      <c r="B88" s="521"/>
+      <c r="C88" s="521"/>
       <c r="D88" s="220">
         <f t="shared" si="14"/>
         <v>5295.9</v>
@@ -46763,11 +46763,11 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="513" t="s">
+      <c r="A89" s="521" t="s">
         <v>335</v>
       </c>
-      <c r="B89" s="513"/>
-      <c r="C89" s="513"/>
+      <c r="B89" s="521"/>
+      <c r="C89" s="521"/>
       <c r="D89" s="220">
         <f t="shared" si="14"/>
         <v>822.27</v>
@@ -46802,11 +46802,11 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="513" t="s">
+      <c r="A90" s="521" t="s">
         <v>331</v>
       </c>
-      <c r="B90" s="513"/>
-      <c r="C90" s="513"/>
+      <c r="B90" s="521"/>
+      <c r="C90" s="521"/>
       <c r="D90" s="220">
         <f t="shared" si="14"/>
         <v>1221</v>
@@ -46841,11 +46841,11 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="513" t="s">
+      <c r="A91" s="521" t="s">
         <v>330</v>
       </c>
-      <c r="B91" s="513"/>
-      <c r="C91" s="513"/>
+      <c r="B91" s="521"/>
+      <c r="C91" s="521"/>
       <c r="D91" s="220">
         <f t="shared" si="14"/>
         <v>718</v>
@@ -46880,11 +46880,11 @@
       </c>
     </row>
     <row r="92" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="513" t="s">
+      <c r="A92" s="521" t="s">
         <v>326</v>
       </c>
-      <c r="B92" s="513"/>
-      <c r="C92" s="513"/>
+      <c r="B92" s="521"/>
+      <c r="C92" s="521"/>
       <c r="D92" s="220">
         <f t="shared" si="14"/>
         <v>1664.88</v>
@@ -46919,11 +46919,11 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="513" t="s">
+      <c r="A93" s="521" t="s">
         <v>325</v>
       </c>
-      <c r="B93" s="513"/>
-      <c r="C93" s="513"/>
+      <c r="B93" s="521"/>
+      <c r="C93" s="521"/>
       <c r="D93" s="220">
         <f t="shared" si="14"/>
         <v>261.05</v>
@@ -46958,11 +46958,11 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="513" t="s">
+      <c r="A94" s="521" t="s">
         <v>324</v>
       </c>
-      <c r="B94" s="513"/>
-      <c r="C94" s="513"/>
+      <c r="B94" s="521"/>
+      <c r="C94" s="521"/>
       <c r="D94" s="220">
         <f t="shared" si="14"/>
         <v>83.22999999999999</v>
@@ -47046,15 +47046,74 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:H12"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:B23"/>
@@ -47071,74 +47130,15 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A60:I60"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A81" r:id="rId1" display="http://www.sasol.com/" xr:uid="{94E57AF8-CF1E-4A4A-992A-3647A9F5048E}"/>

</xml_diff>

<commit_message>
Some tweaks to emissions parameters
</commit_message>
<xml_diff>
--- a/VT_REGION1_REF.xlsx
+++ b/VT_REGION1_REF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468863CF-A6A6-410D-9954-15744A0F2E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED54206E-D22F-404B-A3DD-BE3FAABFB4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{D244279C-3AE9-4D06-974A-1742C2D08212}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -9468,24 +9468,6 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9515,6 +9497,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="13" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="11" borderId="6" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9552,10 +9552,31 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9574,27 +9595,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16922,9 +16922,6 @@
           <cell r="C14" t="str">
             <v>CLE</v>
           </cell>
-          <cell r="AZ14">
-            <v>1E-3</v>
-          </cell>
         </row>
         <row r="15">
           <cell r="B15" t="str">
@@ -16956,12 +16953,6 @@
           </cell>
           <cell r="C18" t="str">
             <v>GAS</v>
-          </cell>
-          <cell r="AY18">
-            <v>56.1</v>
-          </cell>
-          <cell r="AZ18">
-            <v>1E-3</v>
           </cell>
         </row>
         <row r="19">
@@ -18764,10 +18755,10 @@
   <dimension ref="A1:BH117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="8" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4:AC4"/>
+      <selection pane="bottomRight" activeCell="K105" sqref="K105:L106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21789,6 +21780,12 @@
         <f>SUMIF(RefineriesData!$J$13:$J$269,$B40&amp;J$4,RefineriesData!$N$13:$N$269)</f>
         <v>66.311492399999992</v>
       </c>
+      <c r="K40" s="117">
+        <v>0</v>
+      </c>
+      <c r="L40" s="117">
+        <v>0</v>
+      </c>
       <c r="M40" s="466">
         <f>RefineriesData!D243</f>
         <v>6.4894696089818042</v>
@@ -22478,6 +22475,12 @@
       <c r="J50" s="439">
         <f>IFERROR(zar.2010*SUMIF(RefineriesData!$J$13:$J$269,$B50&amp;J$4,RefineriesData!$N$13:$N$269),"")</f>
         <v>55.422377929572328</v>
+      </c>
+      <c r="K50" s="117">
+        <v>0</v>
+      </c>
+      <c r="L50" s="117">
+        <v>0</v>
       </c>
       <c r="M50" s="466">
         <f>M40</f>
@@ -23163,6 +23166,12 @@
         <f>J50</f>
         <v>55.422377929572328</v>
       </c>
+      <c r="K60" s="117">
+        <v>0</v>
+      </c>
+      <c r="L60" s="117">
+        <v>0</v>
+      </c>
       <c r="M60" s="466">
         <f>M40</f>
         <v>6.4894696089818042</v>
@@ -23847,8 +23856,12 @@
         <f>IFERROR(zar.2010*SUMIF(RefineriesData!$J$13:$J$269,$B70&amp;J$4,RefineriesData!$N$13:$N$269),"")</f>
         <v>36.817867655087646</v>
       </c>
-      <c r="K70" s="435"/>
-      <c r="L70" s="435"/>
+      <c r="K70" s="435">
+        <v>0</v>
+      </c>
+      <c r="L70" s="435">
+        <v>0</v>
+      </c>
       <c r="M70" s="435">
         <f>SUMIF(RefineriesData!$J$13:$J$245,$B70&amp;M$5,RefineriesData!$N$13:$N$245)</f>
         <v>109.73413027616279</v>
@@ -24686,8 +24699,12 @@
         <f>IFERROR(zar.2010*SUMIF(RefineriesData!$J$13:$J$269,$B82&amp;J$4,RefineriesData!$N$13:$N$269),"")</f>
         <v>36.817867655087646</v>
       </c>
-      <c r="K82" s="435"/>
-      <c r="L82" s="435"/>
+      <c r="K82" s="435">
+        <v>0</v>
+      </c>
+      <c r="L82" s="435">
+        <v>0</v>
+      </c>
       <c r="M82" s="435">
         <f>SUMIF(RefineriesData!$J$13:$J$245,$B82&amp;M$5,RefineriesData!$N$13:$N$245)</f>
         <v>109.73413027616279</v>
@@ -26263,11 +26280,11 @@
       <c r="I105" s="436"/>
       <c r="J105" s="435"/>
       <c r="K105" s="484">
-        <f>RefineriesData!D33</f>
-        <v>95.428011064048093</v>
-      </c>
-      <c r="L105" s="468">
-        <f>[4]NameConv!$AZ$14/F105</f>
+        <f>96.25/F105</f>
+        <v>113.10501165543117</v>
+      </c>
+      <c r="L105" s="484">
+        <f>0.001/F105</f>
         <v>1.1751170042122719E-3</v>
       </c>
       <c r="M105" s="484"/>
@@ -26340,11 +26357,11 @@
       <c r="I106" s="436"/>
       <c r="J106" s="435"/>
       <c r="K106" s="484">
-        <f>RefineriesData!D31/F106</f>
-        <v>95.428011064048093</v>
-      </c>
-      <c r="L106" s="468">
-        <f>[4]NameConv!$AZ$14/F106</f>
+        <f>96.25/F106</f>
+        <v>113.10501165543117</v>
+      </c>
+      <c r="L106" s="484">
+        <f>0.001/F106</f>
         <v>1.1751170042122719E-3</v>
       </c>
       <c r="M106" s="484"/>
@@ -26414,14 +26431,8 @@
       <c r="H107" s="435"/>
       <c r="I107" s="435"/>
       <c r="J107" s="465"/>
-      <c r="K107" s="484">
-        <f>[4]NameConv!AY18</f>
-        <v>56.1</v>
-      </c>
-      <c r="L107" s="468">
-        <f>[4]NameConv!AZ18</f>
-        <v>1E-3</v>
-      </c>
+      <c r="K107" s="484"/>
+      <c r="L107" s="468"/>
       <c r="M107" s="484"/>
       <c r="N107" s="468"/>
       <c r="P107" s="436"/>
@@ -26550,8 +26561,8 @@
   </sheetPr>
   <dimension ref="A1:AH286"/>
   <sheetViews>
-    <sheetView topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="N267" sqref="N267"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34453,26 +34464,26 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="96" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="486" t="s">
+      <c r="C2" s="496" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="487"/>
-      <c r="E2" s="487"/>
-      <c r="F2" s="488" t="s">
+      <c r="D2" s="497"/>
+      <c r="E2" s="497"/>
+      <c r="F2" s="498" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="489"/>
-      <c r="H2" s="490"/>
-      <c r="I2" s="488" t="s">
+      <c r="G2" s="499"/>
+      <c r="H2" s="500"/>
+      <c r="I2" s="498" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="489"/>
-      <c r="K2" s="490"/>
-      <c r="L2" s="488" t="s">
+      <c r="J2" s="499"/>
+      <c r="K2" s="500"/>
+      <c r="L2" s="498" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="489"/>
-      <c r="N2" s="490"/>
+      <c r="M2" s="499"/>
+      <c r="N2" s="500"/>
       <c r="O2" s="97"/>
       <c r="P2" s="13"/>
       <c r="AA2" s="96" t="s">
@@ -34745,10 +34756,10 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="491" t="s">
+      <c r="A9" s="485" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="492"/>
+      <c r="B9" s="486"/>
       <c r="C9" s="49"/>
       <c r="D9" s="44">
         <f>D5/$O$5</f>
@@ -34773,49 +34784,49 @@
       <c r="O9" s="7">
         <v>788</v>
       </c>
-      <c r="Q9" s="497" t="s">
+      <c r="Q9" s="491" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="499" t="s">
+      <c r="S9" s="493" t="s">
         <v>83</v>
       </c>
-      <c r="V9" s="495" t="s">
+      <c r="V9" s="489" t="s">
         <v>881</v>
       </c>
-      <c r="W9" s="495" t="s">
+      <c r="W9" s="489" t="s">
         <v>882</v>
       </c>
-      <c r="X9" s="495" t="s">
+      <c r="X9" s="489" t="s">
         <v>82</v>
       </c>
-      <c r="Y9" s="495" t="s">
+      <c r="Y9" s="489" t="s">
         <v>883</v>
       </c>
-      <c r="Z9" s="495" t="s">
+      <c r="Z9" s="489" t="s">
         <v>884</v>
       </c>
-      <c r="AA9" s="495" t="s">
+      <c r="AA9" s="489" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="495" t="s">
+      <c r="AB9" s="489" t="s">
         <v>885</v>
       </c>
-      <c r="AC9" s="495" t="s">
+      <c r="AC9" s="489" t="s">
         <v>886</v>
       </c>
-      <c r="AD9" s="495" t="s">
+      <c r="AD9" s="489" t="s">
         <v>80</v>
       </c>
-      <c r="AE9" s="495" t="s">
+      <c r="AE9" s="489" t="s">
         <v>887</v>
       </c>
-      <c r="AF9" s="495" t="s">
+      <c r="AF9" s="489" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="493"/>
-      <c r="B10" s="494"/>
+      <c r="A10" s="487"/>
+      <c r="B10" s="488"/>
       <c r="C10" s="49"/>
       <c r="D10" s="9">
         <f>D9*788</f>
@@ -34841,25 +34852,25 @@
         <f>O9-G10</f>
         <v>422.2729198252656</v>
       </c>
-      <c r="Q10" s="498"/>
+      <c r="Q10" s="492"/>
       <c r="R10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="S10" s="500"/>
+      <c r="S10" s="494"/>
       <c r="U10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="V10" s="496"/>
-      <c r="W10" s="496"/>
-      <c r="X10" s="496"/>
-      <c r="Y10" s="496"/>
-      <c r="Z10" s="496"/>
-      <c r="AA10" s="496"/>
-      <c r="AB10" s="496"/>
-      <c r="AC10" s="496"/>
-      <c r="AD10" s="496"/>
-      <c r="AE10" s="496"/>
-      <c r="AF10" s="496"/>
+      <c r="V10" s="490"/>
+      <c r="W10" s="490"/>
+      <c r="X10" s="490"/>
+      <c r="Y10" s="490"/>
+      <c r="Z10" s="490"/>
+      <c r="AA10" s="490"/>
+      <c r="AB10" s="490"/>
+      <c r="AC10" s="490"/>
+      <c r="AD10" s="490"/>
+      <c r="AE10" s="490"/>
+      <c r="AF10" s="490"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
@@ -37351,11 +37362,11 @@
       <c r="J62" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="485" t="s">
+      <c r="K62" s="495" t="s">
         <v>26</v>
       </c>
-      <c r="L62" s="485"/>
-      <c r="M62" s="485"/>
+      <c r="L62" s="495"/>
+      <c r="M62" s="495"/>
       <c r="N62"/>
     </row>
     <row r="63" spans="3:22" ht="15" x14ac:dyDescent="0.25">
@@ -37613,6 +37624,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AC9:AC10"/>
@@ -37627,11 +37643,6 @@
     <mergeCell ref="AB9:AB10"/>
     <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="W9:W10"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40300,7 +40311,7 @@
         <v>190</v>
       </c>
       <c r="G2" s="509"/>
-      <c r="H2" s="490"/>
+      <c r="H2" s="500"/>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -40542,7 +40553,7 @@
       <c r="G14" s="88"/>
       <c r="H14" s="154"/>
       <c r="I14" s="153"/>
-      <c r="J14" s="500"/>
+      <c r="J14" s="494"/>
       <c r="K14" s="152" t="s">
         <v>79</v>
       </c>
@@ -44430,27 +44441,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="513" t="s">
+      <c r="A1" s="521" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
+      <c r="B1" s="516"/>
+      <c r="C1" s="516"/>
+      <c r="D1" s="516"/>
+      <c r="E1" s="516"/>
+      <c r="F1" s="516"/>
+      <c r="G1" s="516"/>
+      <c r="H1" s="516"/>
+      <c r="I1" s="516"/>
       <c r="J1" s="216" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="515" t="s">
+      <c r="A2" s="522" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="515"/>
-      <c r="C2" s="515"/>
+      <c r="B2" s="522"/>
+      <c r="C2" s="522"/>
       <c r="D2" s="259">
         <v>2019</v>
       </c>
@@ -44487,16 +44498,16 @@
       <c r="U2" s="252"/>
     </row>
     <row r="3" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="516" t="s">
+      <c r="A3" s="523" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="516"/>
+      <c r="B3" s="523"/>
       <c r="C3" s="254"/>
       <c r="D3" s="255"/>
       <c r="E3" s="254"/>
       <c r="F3" s="254"/>
       <c r="G3" s="253"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="524" t="s">
         <v>373</v>
       </c>
       <c r="Q3"/>
@@ -44506,10 +44517,10 @@
       <c r="U3" s="252"/>
     </row>
     <row r="4" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="520" t="s">
+      <c r="A4" s="527" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="520"/>
+      <c r="B4" s="527"/>
       <c r="C4" s="241">
         <v>1</v>
       </c>
@@ -44525,7 +44536,7 @@
       <c r="G4" s="221">
         <v>18806</v>
       </c>
-      <c r="H4" s="518"/>
+      <c r="H4" s="525"/>
       <c r="J4" s="216">
         <f>D4/F4</f>
         <v>0.99859246427024684</v>
@@ -44543,10 +44554,10 @@
       <c r="T4" s="252"/>
     </row>
     <row r="5" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="521" t="s">
+      <c r="A5" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="521"/>
+      <c r="B5" s="513"/>
       <c r="C5" s="239"/>
       <c r="D5" s="231">
         <v>6736</v>
@@ -44560,13 +44571,13 @@
       <c r="G5" s="221">
         <v>7019</v>
       </c>
-      <c r="H5" s="518"/>
+      <c r="H5" s="525"/>
     </row>
     <row r="6" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="521" t="s">
+      <c r="A6" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="521"/>
+      <c r="B6" s="513"/>
       <c r="C6" s="239"/>
       <c r="D6" s="231">
         <v>1467</v>
@@ -44580,13 +44591,13 @@
       <c r="G6" s="221">
         <v>1461</v>
       </c>
-      <c r="H6" s="518"/>
+      <c r="H6" s="525"/>
     </row>
     <row r="7" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="521" t="s">
+      <c r="A7" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="521"/>
+      <c r="B7" s="513"/>
       <c r="C7" s="239"/>
       <c r="D7" s="231">
         <v>3209</v>
@@ -44600,13 +44611,13 @@
       <c r="G7" s="221">
         <v>3331</v>
       </c>
-      <c r="H7" s="518"/>
+      <c r="H7" s="525"/>
     </row>
     <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="521" t="s">
+      <c r="A8" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B8" s="521"/>
+      <c r="B8" s="513"/>
       <c r="C8" s="239"/>
       <c r="D8" s="231">
         <v>4271</v>
@@ -44620,13 +44631,13 @@
       <c r="G8" s="221">
         <v>4067</v>
       </c>
-      <c r="H8" s="518"/>
+      <c r="H8" s="525"/>
     </row>
     <row r="9" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="521" t="s">
+      <c r="A9" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="521"/>
+      <c r="B9" s="513"/>
       <c r="C9" s="239"/>
       <c r="D9" s="231">
         <v>1277</v>
@@ -44640,13 +44651,13 @@
       <c r="G9" s="221">
         <v>1309</v>
       </c>
-      <c r="H9" s="518"/>
+      <c r="H9" s="525"/>
     </row>
     <row r="10" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="521" t="s">
+      <c r="A10" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="521"/>
+      <c r="B10" s="513"/>
       <c r="C10" s="239"/>
       <c r="D10" s="233">
         <v>688</v>
@@ -44660,13 +44671,13 @@
       <c r="G10" s="218">
         <v>793</v>
       </c>
-      <c r="H10" s="518"/>
+      <c r="H10" s="525"/>
     </row>
     <row r="11" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="521" t="s">
+      <c r="A11" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="521"/>
+      <c r="B11" s="513"/>
       <c r="C11" s="239"/>
       <c r="D11" s="233">
         <v>53</v>
@@ -44680,14 +44691,14 @@
       <c r="G11" s="218">
         <v>62</v>
       </c>
-      <c r="H11" s="518"/>
+      <c r="H11" s="525"/>
     </row>
     <row r="12" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="522" t="s">
+      <c r="A12" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B12" s="522"/>
-      <c r="C12" s="522"/>
+      <c r="B12" s="514"/>
+      <c r="C12" s="514"/>
       <c r="D12" s="251">
         <v>745</v>
       </c>
@@ -44700,14 +44711,14 @@
       <c r="G12" s="249">
         <v>763</v>
       </c>
-      <c r="H12" s="519"/>
+      <c r="H12" s="526"/>
       <c r="V12" s="243"/>
     </row>
     <row r="13" spans="1:22" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="523" t="s">
+      <c r="A13" s="520" t="s">
         <v>396</v>
       </c>
-      <c r="B13" s="523"/>
+      <c r="B13" s="520"/>
       <c r="C13" s="248">
         <v>2</v>
       </c>
@@ -44719,10 +44730,10 @@
       <c r="V13" s="243"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="514" t="s">
+      <c r="A14" s="516" t="s">
         <v>395</v>
       </c>
-      <c r="B14" s="514"/>
+      <c r="B14" s="516"/>
       <c r="C14" s="239"/>
       <c r="D14" s="231">
         <v>105.04</v>
@@ -44757,10 +44768,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="521" t="s">
+      <c r="A15" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="521"/>
+      <c r="B15" s="513"/>
       <c r="C15" s="239"/>
       <c r="D15" s="231">
         <v>96.16</v>
@@ -44793,10 +44804,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="521" t="s">
+      <c r="A16" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B16" s="521"/>
+      <c r="B16" s="513"/>
       <c r="C16" s="239"/>
       <c r="D16" s="231">
         <v>5.34</v>
@@ -44829,10 +44840,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="521" t="s">
+      <c r="A17" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B17" s="521"/>
+      <c r="B17" s="513"/>
       <c r="C17" s="239"/>
       <c r="D17" s="231">
         <v>3.49</v>
@@ -44865,10 +44876,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="521" t="s">
+      <c r="A18" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B18" s="521"/>
+      <c r="B18" s="513"/>
       <c r="C18" s="239"/>
       <c r="D18" s="242">
         <v>0</v>
@@ -44901,10 +44912,10 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="521" t="s">
+      <c r="A19" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="521"/>
+      <c r="B19" s="513"/>
       <c r="C19" s="239"/>
       <c r="D19" s="231">
         <v>0</v>
@@ -44937,10 +44948,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="521" t="s">
+      <c r="A20" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B20" s="521"/>
+      <c r="B20" s="513"/>
       <c r="C20" s="239"/>
       <c r="D20" s="231">
         <v>0.04</v>
@@ -44973,10 +44984,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="521" t="s">
+      <c r="A21" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B21" s="521"/>
+      <c r="B21" s="513"/>
       <c r="C21" s="239"/>
       <c r="D21" s="231">
         <v>0</v>
@@ -45009,11 +45020,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="521" t="s">
+      <c r="A22" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B22" s="521"/>
-      <c r="C22" s="521"/>
+      <c r="B22" s="513"/>
+      <c r="C22" s="513"/>
       <c r="D22" s="231">
         <v>0.01</v>
       </c>
@@ -45045,10 +45056,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="514" t="s">
+      <c r="A23" s="516" t="s">
         <v>394</v>
       </c>
-      <c r="B23" s="514"/>
+      <c r="B23" s="516"/>
       <c r="C23" s="239"/>
       <c r="D23" s="231">
         <v>1.64</v>
@@ -45083,10 +45094,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="521" t="s">
+      <c r="A24" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B24" s="521"/>
+      <c r="B24" s="513"/>
       <c r="C24" s="239"/>
       <c r="D24" s="231">
         <v>0.9</v>
@@ -45119,10 +45130,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="521" t="s">
+      <c r="A25" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="521"/>
+      <c r="B25" s="513"/>
       <c r="C25" s="239"/>
       <c r="D25" s="231">
         <v>0.73</v>
@@ -45155,10 +45166,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="521" t="s">
+      <c r="A26" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B26" s="521"/>
+      <c r="B26" s="513"/>
       <c r="C26" s="239"/>
       <c r="D26" s="231">
         <v>0</v>
@@ -45191,10 +45202,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="521" t="s">
+      <c r="A27" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B27" s="521"/>
+      <c r="B27" s="513"/>
       <c r="C27" s="239"/>
       <c r="D27" s="231">
         <v>0</v>
@@ -45227,10 +45238,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="521" t="s">
+      <c r="A28" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="521"/>
+      <c r="B28" s="513"/>
       <c r="C28" s="239"/>
       <c r="D28" s="231">
         <v>0</v>
@@ -45263,10 +45274,10 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="521" t="s">
+      <c r="A29" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B29" s="521"/>
+      <c r="B29" s="513"/>
       <c r="C29" s="239"/>
       <c r="D29" s="231">
         <v>0.01</v>
@@ -45299,10 +45310,10 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="521" t="s">
+      <c r="A30" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B30" s="521"/>
+      <c r="B30" s="513"/>
       <c r="C30" s="239"/>
       <c r="D30" s="231">
         <v>0</v>
@@ -45335,11 +45346,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="521" t="s">
+      <c r="A31" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B31" s="521"/>
-      <c r="C31" s="521"/>
+      <c r="B31" s="513"/>
+      <c r="C31" s="513"/>
       <c r="D31" s="231">
         <v>0</v>
       </c>
@@ -45371,10 +45382,10 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="514" t="s">
+      <c r="A32" s="516" t="s">
         <v>393</v>
       </c>
-      <c r="B32" s="514"/>
+      <c r="B32" s="516"/>
       <c r="C32" s="239"/>
       <c r="D32" s="231">
         <v>56004</v>
@@ -45409,10 +45420,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="521" t="s">
+      <c r="A33" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B33" s="521"/>
+      <c r="B33" s="513"/>
       <c r="C33" s="239"/>
       <c r="D33" s="231">
         <v>48418</v>
@@ -45451,10 +45462,10 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="521" t="s">
+      <c r="A34" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="521"/>
+      <c r="B34" s="513"/>
       <c r="C34" s="239"/>
       <c r="D34" s="231">
         <v>4557</v>
@@ -45487,10 +45498,10 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="521" t="s">
+      <c r="A35" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B35" s="521"/>
+      <c r="B35" s="513"/>
       <c r="C35" s="239"/>
       <c r="D35" s="233">
         <v>16</v>
@@ -45523,10 +45534,10 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="521" t="s">
+      <c r="A36" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B36" s="521"/>
+      <c r="B36" s="513"/>
       <c r="C36" s="239"/>
       <c r="D36" s="233">
         <v>932</v>
@@ -45559,10 +45570,10 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="521" t="s">
+      <c r="A37" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B37" s="521"/>
+      <c r="B37" s="513"/>
       <c r="C37" s="239"/>
       <c r="D37" s="233">
         <v>610</v>
@@ -45595,10 +45606,10 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="521" t="s">
+      <c r="A38" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="521"/>
+      <c r="B38" s="513"/>
       <c r="C38" s="239"/>
       <c r="D38" s="231">
         <v>1163</v>
@@ -45631,10 +45642,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="521" t="s">
+      <c r="A39" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B39" s="521"/>
+      <c r="B39" s="513"/>
       <c r="C39" s="239"/>
       <c r="D39" s="233">
         <v>261</v>
@@ -45667,11 +45678,11 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="521" t="s">
+      <c r="A40" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B40" s="521"/>
-      <c r="C40" s="521"/>
+      <c r="B40" s="513"/>
+      <c r="C40" s="513"/>
       <c r="D40" s="233">
         <v>47</v>
       </c>
@@ -45703,10 +45714,10 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="514" t="s">
+      <c r="A41" s="516" t="s">
         <v>391</v>
       </c>
-      <c r="B41" s="514"/>
+      <c r="B41" s="516"/>
       <c r="C41" s="241">
         <v>3</v>
       </c>
@@ -45727,10 +45738,10 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="521" t="s">
+      <c r="A42" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B42" s="521"/>
+      <c r="B42" s="513"/>
       <c r="C42" s="239"/>
       <c r="D42" s="231">
         <v>5596</v>
@@ -45766,10 +45777,10 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="521" t="s">
+      <c r="A43" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="521"/>
+      <c r="B43" s="513"/>
       <c r="C43" s="239"/>
       <c r="D43" s="233">
         <v>400</v>
@@ -45805,10 +45816,10 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="521" t="s">
+      <c r="A44" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B44" s="521"/>
+      <c r="B44" s="513"/>
       <c r="C44" s="239"/>
       <c r="D44" s="233">
         <v>726</v>
@@ -45844,10 +45855,10 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="521" t="s">
+      <c r="A45" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="521"/>
+      <c r="B45" s="513"/>
       <c r="C45" s="239"/>
       <c r="D45" s="233">
         <v>289</v>
@@ -45883,10 +45894,10 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="521" t="s">
+      <c r="A46" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B46" s="521"/>
+      <c r="B46" s="513"/>
       <c r="C46" s="239"/>
       <c r="D46" s="233">
         <v>108</v>
@@ -45903,10 +45914,10 @@
       <c r="H46" s="230"/>
     </row>
     <row r="47" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="521" t="s">
+      <c r="A47" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="521"/>
+      <c r="B47" s="513"/>
       <c r="C47" s="239"/>
       <c r="D47" s="233">
         <v>498</v>
@@ -45923,10 +45934,10 @@
       <c r="H47" s="230"/>
     </row>
     <row r="48" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="521" t="s">
+      <c r="A48" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="521"/>
+      <c r="B48" s="513"/>
       <c r="C48" s="239"/>
       <c r="D48" s="231">
         <v>0</v>
@@ -45943,11 +45954,11 @@
       <c r="H48" s="230"/>
     </row>
     <row r="49" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="521" t="s">
+      <c r="A49" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="521"/>
-      <c r="C49" s="521"/>
+      <c r="B49" s="513"/>
+      <c r="C49" s="513"/>
       <c r="D49" s="233">
         <v>36</v>
       </c>
@@ -45963,10 +45974,10 @@
       <c r="H49" s="230"/>
     </row>
     <row r="50" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="514" t="s">
+      <c r="A50" s="516" t="s">
         <v>390</v>
       </c>
-      <c r="B50" s="514"/>
+      <c r="B50" s="516"/>
       <c r="C50" s="241">
         <v>4</v>
       </c>
@@ -45987,10 +45998,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="521" t="s">
+      <c r="A51" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B51" s="521"/>
+      <c r="B51" s="513"/>
       <c r="C51" s="239"/>
       <c r="D51" s="231">
         <v>0</v>
@@ -46007,10 +46018,10 @@
       <c r="H51" s="230"/>
     </row>
     <row r="52" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="521" t="s">
+      <c r="A52" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B52" s="521"/>
+      <c r="B52" s="513"/>
       <c r="C52" s="239"/>
       <c r="D52" s="231">
         <v>0</v>
@@ -46027,10 +46038,10 @@
       <c r="H52" s="230"/>
     </row>
     <row r="53" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="521" t="s">
+      <c r="A53" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B53" s="521"/>
+      <c r="B53" s="513"/>
       <c r="C53" s="239"/>
       <c r="D53" s="231">
         <v>0</v>
@@ -46047,10 +46058,10 @@
       <c r="H53" s="230"/>
     </row>
     <row r="54" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="521" t="s">
+      <c r="A54" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B54" s="521"/>
+      <c r="B54" s="513"/>
       <c r="C54" s="239"/>
       <c r="D54" s="231">
         <v>0</v>
@@ -46067,10 +46078,10 @@
       <c r="H54" s="230"/>
     </row>
     <row r="55" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="521" t="s">
+      <c r="A55" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B55" s="521"/>
+      <c r="B55" s="513"/>
       <c r="C55" s="239"/>
       <c r="D55" s="231">
         <v>0</v>
@@ -46087,10 +46098,10 @@
       <c r="H55" s="230"/>
     </row>
     <row r="56" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="521" t="s">
+      <c r="A56" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B56" s="521"/>
+      <c r="B56" s="513"/>
       <c r="C56" s="239"/>
       <c r="D56" s="231">
         <v>0</v>
@@ -46107,10 +46118,10 @@
       <c r="H56" s="230"/>
     </row>
     <row r="57" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="521" t="s">
+      <c r="A57" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="521"/>
+      <c r="B57" s="513"/>
       <c r="C57" s="239"/>
       <c r="D57" s="231">
         <v>0.05</v>
@@ -46127,11 +46138,11 @@
       <c r="H57" s="230"/>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="522" t="s">
+      <c r="A58" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B58" s="522"/>
-      <c r="C58" s="522"/>
+      <c r="B58" s="514"/>
+      <c r="C58" s="514"/>
       <c r="D58" s="229">
         <v>0</v>
       </c>
@@ -46147,46 +46158,46 @@
       <c r="H58" s="238"/>
     </row>
     <row r="59" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="514"/>
-      <c r="B59" s="514"/>
-      <c r="C59" s="514"/>
-      <c r="D59" s="514"/>
-      <c r="E59" s="514"/>
-      <c r="F59" s="514"/>
-      <c r="G59" s="514"/>
-      <c r="H59" s="514"/>
-      <c r="I59" s="514"/>
+      <c r="A59" s="516"/>
+      <c r="B59" s="516"/>
+      <c r="C59" s="516"/>
+      <c r="D59" s="516"/>
+      <c r="E59" s="516"/>
+      <c r="F59" s="516"/>
+      <c r="G59" s="516"/>
+      <c r="H59" s="516"/>
+      <c r="I59" s="516"/>
     </row>
     <row r="60" spans="1:9" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="514"/>
-      <c r="B60" s="514"/>
-      <c r="C60" s="514"/>
-      <c r="D60" s="514"/>
-      <c r="E60" s="514"/>
-      <c r="F60" s="514"/>
-      <c r="G60" s="514"/>
-      <c r="H60" s="514"/>
-      <c r="I60" s="514"/>
+      <c r="A60" s="516"/>
+      <c r="B60" s="516"/>
+      <c r="C60" s="516"/>
+      <c r="D60" s="516"/>
+      <c r="E60" s="516"/>
+      <c r="F60" s="516"/>
+      <c r="G60" s="516"/>
+      <c r="H60" s="516"/>
+      <c r="I60" s="516"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="524" t="s">
+      <c r="A61" s="519" t="s">
         <v>388</v>
       </c>
-      <c r="B61" s="524"/>
-      <c r="C61" s="524"/>
-      <c r="D61" s="524"/>
-      <c r="E61" s="524"/>
-      <c r="F61" s="524"/>
-      <c r="G61" s="524"/>
-      <c r="H61" s="524"/>
-      <c r="I61" s="524"/>
+      <c r="B61" s="519"/>
+      <c r="C61" s="519"/>
+      <c r="D61" s="519"/>
+      <c r="E61" s="519"/>
+      <c r="F61" s="519"/>
+      <c r="G61" s="519"/>
+      <c r="H61" s="519"/>
+      <c r="I61" s="519"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="525" t="s">
+      <c r="A62" s="517" t="s">
         <v>345</v>
       </c>
-      <c r="B62" s="525"/>
-      <c r="C62" s="525"/>
+      <c r="B62" s="517"/>
+      <c r="C62" s="517"/>
       <c r="D62" s="225">
         <v>2019</v>
       </c>
@@ -46204,11 +46215,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="526" t="s">
+      <c r="A63" s="518" t="s">
         <v>344</v>
       </c>
-      <c r="B63" s="526"/>
-      <c r="C63" s="526"/>
+      <c r="B63" s="518"/>
+      <c r="C63" s="518"/>
       <c r="D63" s="220" t="s">
         <v>386</v>
       </c>
@@ -46226,11 +46237,11 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="521" t="s">
+      <c r="A64" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="521"/>
-      <c r="C64" s="521"/>
+      <c r="B64" s="513"/>
+      <c r="C64" s="513"/>
       <c r="D64" s="231" t="s">
         <v>382</v>
       </c>
@@ -46246,11 +46257,11 @@
       <c r="H64" s="230"/>
     </row>
     <row r="65" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="521" t="s">
+      <c r="A65" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B65" s="521"/>
-      <c r="C65" s="521"/>
+      <c r="B65" s="513"/>
+      <c r="C65" s="513"/>
       <c r="D65" s="231" t="s">
         <v>380</v>
       </c>
@@ -46266,11 +46277,11 @@
       <c r="H65" s="230"/>
     </row>
     <row r="66" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="521" t="s">
+      <c r="A66" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B66" s="521"/>
-      <c r="C66" s="521"/>
+      <c r="B66" s="513"/>
+      <c r="C66" s="513"/>
       <c r="D66" s="233">
         <v>822</v>
       </c>
@@ -46286,11 +46297,11 @@
       <c r="H66" s="230"/>
     </row>
     <row r="67" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="521" t="s">
+      <c r="A67" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B67" s="521"/>
-      <c r="C67" s="521"/>
+      <c r="B67" s="513"/>
+      <c r="C67" s="513"/>
       <c r="D67" s="231" t="s">
         <v>379</v>
       </c>
@@ -46306,11 +46317,11 @@
       <c r="H67" s="230"/>
     </row>
     <row r="68" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="521" t="s">
+      <c r="A68" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="521"/>
-      <c r="C68" s="521"/>
+      <c r="B68" s="513"/>
+      <c r="C68" s="513"/>
       <c r="D68" s="233">
         <v>717</v>
       </c>
@@ -46326,11 +46337,11 @@
       <c r="H68" s="230"/>
     </row>
     <row r="69" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="521" t="s">
+      <c r="A69" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="521"/>
-      <c r="C69" s="521"/>
+      <c r="B69" s="513"/>
+      <c r="C69" s="513"/>
       <c r="D69" s="231" t="s">
         <v>378</v>
       </c>
@@ -46346,11 +46357,11 @@
       <c r="H69" s="230"/>
     </row>
     <row r="70" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="521" t="s">
+      <c r="A70" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B70" s="521"/>
-      <c r="C70" s="521"/>
+      <c r="B70" s="513"/>
+      <c r="C70" s="513"/>
       <c r="D70" s="233">
         <v>261</v>
       </c>
@@ -46366,11 +46377,11 @@
       <c r="H70" s="230"/>
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="521" t="s">
+      <c r="A71" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B71" s="521"/>
-      <c r="C71" s="521"/>
+      <c r="B71" s="513"/>
+      <c r="C71" s="513"/>
       <c r="D71" s="233">
         <v>83</v>
       </c>
@@ -46386,11 +46397,11 @@
       <c r="H71" s="230"/>
     </row>
     <row r="72" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="514" t="s">
+      <c r="A72" s="516" t="s">
         <v>377</v>
       </c>
-      <c r="B72" s="514"/>
-      <c r="C72" s="514"/>
+      <c r="B72" s="516"/>
+      <c r="C72" s="516"/>
       <c r="D72" s="231" t="s">
         <v>368</v>
       </c>
@@ -46408,11 +46419,11 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="521" t="s">
+      <c r="A73" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B73" s="521"/>
-      <c r="C73" s="521"/>
+      <c r="B73" s="513"/>
+      <c r="C73" s="513"/>
       <c r="D73" s="231" t="s">
         <v>372</v>
       </c>
@@ -46428,11 +46439,11 @@
       <c r="H73" s="230"/>
     </row>
     <row r="74" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="521" t="s">
+      <c r="A74" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B74" s="521"/>
-      <c r="C74" s="521"/>
+      <c r="B74" s="513"/>
+      <c r="C74" s="513"/>
       <c r="D74" s="231" t="s">
         <v>368</v>
       </c>
@@ -46448,11 +46459,11 @@
       <c r="H74" s="230"/>
     </row>
     <row r="75" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="521" t="s">
+      <c r="A75" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B75" s="521"/>
-      <c r="C75" s="521"/>
+      <c r="B75" s="513"/>
+      <c r="C75" s="513"/>
       <c r="D75" s="231" t="s">
         <v>348</v>
       </c>
@@ -46468,11 +46479,11 @@
       <c r="H75" s="230"/>
     </row>
     <row r="76" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="521" t="s">
+      <c r="A76" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B76" s="521"/>
-      <c r="C76" s="521"/>
+      <c r="B76" s="513"/>
+      <c r="C76" s="513"/>
       <c r="D76" s="231" t="s">
         <v>362</v>
       </c>
@@ -46488,11 +46499,11 @@
       <c r="H76" s="230"/>
     </row>
     <row r="77" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="521" t="s">
+      <c r="A77" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B77" s="521"/>
-      <c r="C77" s="521"/>
+      <c r="B77" s="513"/>
+      <c r="C77" s="513"/>
       <c r="D77" s="231" t="s">
         <v>361</v>
       </c>
@@ -46508,11 +46519,11 @@
       <c r="H77" s="230"/>
     </row>
     <row r="78" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="521" t="s">
+      <c r="A78" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B78" s="521"/>
-      <c r="C78" s="521"/>
+      <c r="B78" s="513"/>
+      <c r="C78" s="513"/>
       <c r="D78" s="231" t="s">
         <v>358</v>
       </c>
@@ -46528,11 +46539,11 @@
       <c r="H78" s="230"/>
     </row>
     <row r="79" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="521" t="s">
+      <c r="A79" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="521"/>
-      <c r="C79" s="521"/>
+      <c r="B79" s="513"/>
+      <c r="C79" s="513"/>
       <c r="D79" s="231" t="s">
         <v>354</v>
       </c>
@@ -46548,11 +46559,11 @@
       <c r="H79" s="230"/>
     </row>
     <row r="80" spans="1:8" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="522" t="s">
+      <c r="A80" s="514" t="s">
         <v>324</v>
       </c>
-      <c r="B80" s="522"/>
-      <c r="C80" s="522"/>
+      <c r="B80" s="514"/>
+      <c r="C80" s="514"/>
       <c r="D80" s="229" t="s">
         <v>349</v>
       </c>
@@ -46568,30 +46579,30 @@
       <c r="H80" s="226"/>
     </row>
     <row r="81" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="527" t="s">
+      <c r="A81" s="515" t="s">
         <v>347</v>
       </c>
-      <c r="B81" s="514"/>
-      <c r="C81" s="514"/>
-      <c r="D81" s="514"/>
-      <c r="E81" s="514"/>
-      <c r="F81" s="514"/>
-      <c r="G81" s="514"/>
-      <c r="H81" s="514"/>
-      <c r="I81" s="514"/>
+      <c r="B81" s="516"/>
+      <c r="C81" s="516"/>
+      <c r="D81" s="516"/>
+      <c r="E81" s="516"/>
+      <c r="F81" s="516"/>
+      <c r="G81" s="516"/>
+      <c r="H81" s="516"/>
+      <c r="I81" s="516"/>
     </row>
     <row r="82" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="514" t="s">
+      <c r="A82" s="516" t="s">
         <v>346</v>
       </c>
-      <c r="B82" s="514"/>
-      <c r="C82" s="514"/>
-      <c r="D82" s="514"/>
-      <c r="E82" s="514"/>
-      <c r="F82" s="514"/>
-      <c r="G82" s="514"/>
-      <c r="H82" s="514"/>
-      <c r="I82" s="514"/>
+      <c r="B82" s="516"/>
+      <c r="C82" s="516"/>
+      <c r="D82" s="516"/>
+      <c r="E82" s="516"/>
+      <c r="F82" s="516"/>
+      <c r="G82" s="516"/>
+      <c r="H82" s="516"/>
+      <c r="I82" s="516"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D83" s="216" t="str">
@@ -46612,11 +46623,11 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="525" t="s">
+      <c r="A85" s="517" t="s">
         <v>345</v>
       </c>
-      <c r="B85" s="525"/>
-      <c r="C85" s="525"/>
+      <c r="B85" s="517"/>
+      <c r="C85" s="517"/>
       <c r="D85" s="225">
         <v>2019</v>
       </c>
@@ -46643,11 +46654,11 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="526" t="s">
+      <c r="A86" s="518" t="s">
         <v>344</v>
       </c>
-      <c r="B86" s="526"/>
-      <c r="C86" s="526"/>
+      <c r="B86" s="518"/>
+      <c r="C86" s="518"/>
       <c r="D86" s="220">
         <f>D14*gwpch4+D23*gwpn2o+D32+D41+D50</f>
         <v>66558.41</v>
@@ -46685,11 +46696,11 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="521" t="s">
+      <c r="A87" s="513" t="s">
         <v>340</v>
       </c>
-      <c r="B87" s="521"/>
-      <c r="C87" s="521"/>
+      <c r="B87" s="513"/>
+      <c r="C87" s="513"/>
       <c r="D87" s="220">
         <f t="shared" ref="D87:D94" si="14">D15*gwpch4+D24*gwpn2o+D33+D42+D51</f>
         <v>56492.08</v>
@@ -46724,11 +46735,11 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="521" t="s">
+      <c r="A88" s="513" t="s">
         <v>336</v>
       </c>
-      <c r="B88" s="521"/>
-      <c r="C88" s="521"/>
+      <c r="B88" s="513"/>
+      <c r="C88" s="513"/>
       <c r="D88" s="220">
         <f t="shared" si="14"/>
         <v>5295.9</v>
@@ -46763,11 +46774,11 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="521" t="s">
+      <c r="A89" s="513" t="s">
         <v>335</v>
       </c>
-      <c r="B89" s="521"/>
-      <c r="C89" s="521"/>
+      <c r="B89" s="513"/>
+      <c r="C89" s="513"/>
       <c r="D89" s="220">
         <f t="shared" si="14"/>
         <v>822.27</v>
@@ -46802,11 +46813,11 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="521" t="s">
+      <c r="A90" s="513" t="s">
         <v>331</v>
       </c>
-      <c r="B90" s="521"/>
-      <c r="C90" s="521"/>
+      <c r="B90" s="513"/>
+      <c r="C90" s="513"/>
       <c r="D90" s="220">
         <f t="shared" si="14"/>
         <v>1221</v>
@@ -46841,11 +46852,11 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="521" t="s">
+      <c r="A91" s="513" t="s">
         <v>330</v>
       </c>
-      <c r="B91" s="521"/>
-      <c r="C91" s="521"/>
+      <c r="B91" s="513"/>
+      <c r="C91" s="513"/>
       <c r="D91" s="220">
         <f t="shared" si="14"/>
         <v>718</v>
@@ -46880,11 +46891,11 @@
       </c>
     </row>
     <row r="92" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="521" t="s">
+      <c r="A92" s="513" t="s">
         <v>326</v>
       </c>
-      <c r="B92" s="521"/>
-      <c r="C92" s="521"/>
+      <c r="B92" s="513"/>
+      <c r="C92" s="513"/>
       <c r="D92" s="220">
         <f t="shared" si="14"/>
         <v>1664.88</v>
@@ -46919,11 +46930,11 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="521" t="s">
+      <c r="A93" s="513" t="s">
         <v>325</v>
       </c>
-      <c r="B93" s="521"/>
-      <c r="C93" s="521"/>
+      <c r="B93" s="513"/>
+      <c r="C93" s="513"/>
       <c r="D93" s="220">
         <f t="shared" si="14"/>
         <v>261.05</v>
@@ -46958,11 +46969,11 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="521" t="s">
+      <c r="A94" s="513" t="s">
         <v>324</v>
       </c>
-      <c r="B94" s="521"/>
-      <c r="C94" s="521"/>
+      <c r="B94" s="513"/>
+      <c r="C94" s="513"/>
       <c r="D94" s="220">
         <f t="shared" si="14"/>
         <v>83.22999999999999</v>
@@ -47046,38 +47057,51 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A94:C94"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="A59:I59"/>
@@ -47094,51 +47118,38 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:H12"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A94:C94"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A81" r:id="rId1" display="http://www.sasol.com/" xr:uid="{94E57AF8-CF1E-4A4A-992A-3647A9F5048E}"/>

</xml_diff>